<commit_message>
Add abilities notes to excel file
</commit_message>
<xml_diff>
--- a/Excel/BotBuilder 2.0.xlsx
+++ b/Excel/BotBuilder 2.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SJWDa\Documents\Creative Projects\Fragment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SJWDa\Projects\Fragment\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129F49A3-A33E-4E48-A7BF-B1C49EC50DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C35A22-B32C-49E9-9073-032FBC62DFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8281E10D-33EF-4D46-A534-1BAF9E624D7F}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="230">
   <si>
     <t>Name</t>
   </si>
@@ -681,28 +681,85 @@
     <t>Blaze</t>
   </si>
   <si>
-    <t>Gain the remaining PPs when you mine an adjacent Fossil Fuel resource</t>
-  </si>
-  <si>
     <t>Frack</t>
   </si>
   <si>
-    <t>10 dmg to random enemy each time this bot attacks</t>
-  </si>
-  <si>
-    <t>Digest</t>
-  </si>
-  <si>
-    <t>Final Form</t>
-  </si>
-  <si>
     <t>Research</t>
   </si>
   <si>
-    <t>Deplete</t>
-  </si>
-  <si>
     <t>Rain recollection</t>
+  </si>
+  <si>
+    <t>Coded?</t>
+  </si>
+  <si>
+    <t>Sync</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Partially</t>
+  </si>
+  <si>
+    <t>Circle back</t>
+  </si>
+  <si>
+    <t>When you would draw a card, draw an extra one</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Agile</t>
+  </si>
+  <si>
+    <t>Disruption</t>
+  </si>
+  <si>
+    <t>Radiate</t>
+  </si>
+  <si>
+    <t>1 dmg to random enemy each time this bot attacks</t>
+  </si>
+  <si>
+    <t>Tinder</t>
+  </si>
+  <si>
+    <t>Gain 4 PP when you mine an adjacent Fossil Fuel resource</t>
+  </si>
+  <si>
+    <t>Lightning</t>
+  </si>
+  <si>
+    <t>Refraction</t>
+  </si>
+  <si>
+    <t>Replenish</t>
+  </si>
+  <si>
+    <t>Streamline</t>
+  </si>
+  <si>
+    <t>Mechanic cards cost 1 less PP to play</t>
+  </si>
+  <si>
+    <t>Recycle</t>
+  </si>
+  <si>
+    <t>When this bot would be sent to the discard pile, send it to your hand instead</t>
+  </si>
+  <si>
+    <t>Repair</t>
+  </si>
+  <si>
+    <t>Mechanic cards heal 1 more HP</t>
+  </si>
+  <si>
+    <t>Downgrade</t>
+  </si>
+  <si>
+    <t>Mechanic cards deal 1 more damage</t>
   </si>
 </sst>
 </file>
@@ -1006,15 +1063,7 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1027,12 +1076,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="139">
+  <dxfs count="140">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2976,15 +3043,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2A520CC-7367-4AD6-BBB5-938EC4DD5652}" name="Table4" displayName="Table4" ref="A1:C24" totalsRowShown="0">
-  <autoFilter ref="A1:C24" xr:uid="{D2A520CC-7367-4AD6-BBB5-938EC4DD5652}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C23">
-    <sortCondition ref="B1:B23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{AA4FFB97-BBFF-4ED6-9160-F33B172F4FDE}" name="Table48" displayName="Table48" ref="A1:E30" totalsRowShown="0">
+  <autoFilter ref="A1:E30" xr:uid="{AA4FFB97-BBFF-4ED6-9160-F33B172F4FDE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E30">
+    <sortCondition ref="B1:B30"/>
   </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{277B50FB-5304-4880-B617-1ACBF4D17975}" name="Ability"/>
-    <tableColumn id="3" xr3:uid="{F3377A5A-BD37-4531-8F37-7929BF4840CF}" name="Type"/>
-    <tableColumn id="2" xr3:uid="{C40B86F4-A261-454C-A38C-7EEDC57BBBA3}" name="Effect"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{02160524-721D-43B6-97F3-4B7CA7F9A9F1}" name="Ability"/>
+    <tableColumn id="3" xr3:uid="{D3F9DE45-C810-4B03-A645-9242A754D326}" name="Type"/>
+    <tableColumn id="4" xr3:uid="{40A98505-3487-4940-B83B-95AE531D08E3}" name="Cost"/>
+    <tableColumn id="2" xr3:uid="{1F852B4E-3AA5-4872-A228-45ABE0CAE6F7}" name="Effect"/>
+    <tableColumn id="5" xr3:uid="{68742C5F-C20A-4A87-ABC5-6F0A1FE7B8C4}" name="Coded?"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2995,16 +3064,16 @@
   <autoFilter ref="A1:Q7" xr:uid="{3FAA1044-8AEB-4310-B12B-1961BF440AB5}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{ABACA6C5-D5B7-485A-BC77-3A9C1EF55782}" name="Type"/>
-    <tableColumn id="2" xr3:uid="{98DBF1C9-36B3-457C-864F-594F9B4A43F9}" name="Generator" dataDxfId="10">
+    <tableColumn id="2" xr3:uid="{98DBF1C9-36B3-457C-864F-594F9B4A43F9}" name="Generator" dataDxfId="11">
       <calculatedColumnFormula array="1">INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table8[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table8[[#This Row],[Type]])+1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FC5D1622-0FC8-4A00-8958-9A4F98C2C4A3}" name="Frame" dataDxfId="9">
+    <tableColumn id="3" xr3:uid="{FC5D1622-0FC8-4A00-8958-9A4F98C2C4A3}" name="Frame" dataDxfId="10">
       <calculatedColumnFormula array="1">INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table8[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table8[[#This Row],[Type]])+1)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{DB7035C1-3C3A-4574-9174-299FCD6046BE}" name="Name">
       <calculatedColumnFormula>_xlfn.CONCAT(B2,C2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B5ED832F-A98B-4E4D-B1BF-CEFAFBF20091}" name="Cost" dataDxfId="8">
+    <tableColumn id="9" xr3:uid="{B5ED832F-A98B-4E4D-B1BF-CEFAFBF20091}" name="Cost" dataDxfId="9">
       <calculatedColumnFormula>SUM(_xlfn.XLOOKUP(Table8[[#This Row],[Generator]],Table2[Name],Table2[Cost]),_xlfn.XLOOKUP(Table8[[#This Row],[Frame]],Table1[Name],Table1[Cost]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{5FBA6BAB-A94C-4CA0-A545-F10CD5101759}" name="PP">
@@ -3019,28 +3088,28 @@
     <tableColumn id="8" xr3:uid="{D892DF1C-8138-4EB4-8C4C-A6F7B91F63C4}" name="Ability 2">
       <calculatedColumnFormula>_xlfn.XLOOKUP(C2,Table1[Name],Table1[Ability])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{621F2675-DA39-4950-BD2E-A247E9053807}" name="Power/Cost" dataDxfId="7">
+    <tableColumn id="16" xr3:uid="{621F2675-DA39-4950-BD2E-A247E9053807}" name="Power/Cost" dataDxfId="8">
       <calculatedColumnFormula>(Table8[[#This Row],[PP]]+(Table8[[#This Row],[HP]]/2)+IF(Table8[[#This Row],[Ability 1]]=0,0,1)+IF(Table8[[#This Row],[Ability 2]]=0,0,1))/(Table8[[#This Row],[Cost]]+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1043AF08-BB57-45E8-B3CF-7FB7430E40B1}" name="Part 1" dataDxfId="6">
+    <tableColumn id="10" xr3:uid="{1043AF08-BB57-45E8-B3CF-7FB7430E40B1}" name="Part 1" dataDxfId="7">
       <calculatedColumnFormula array="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{109CDE57-0F48-4932-B7BE-EAE14DBBDEB2}" name="Name2" dataDxfId="5">
+    <tableColumn id="11" xr3:uid="{109CDE57-0F48-4932-B7BE-EAE14DBBDEB2}" name="Name2" dataDxfId="6">
       <calculatedColumnFormula>_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{61864B2F-DDDC-4DBA-890D-CE1EC3F23BE7}" name="Cost2" dataDxfId="4">
+    <tableColumn id="12" xr3:uid="{61864B2F-DDDC-4DBA-890D-CE1EC3F23BE7}" name="Cost2" dataDxfId="5">
       <calculatedColumnFormula>SUM(Table8[[#This Row],[Cost]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Cost]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{FECCECFA-E3F9-4DA5-9AC1-015032FEDEB9}" name="PP2" dataDxfId="3">
+    <tableColumn id="13" xr3:uid="{FECCECFA-E3F9-4DA5-9AC1-015032FEDEB9}" name="PP2" dataDxfId="4">
       <calculatedColumnFormula>SUM(Table8[[#This Row],[PP]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[PP]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6E9D2E4F-4D5A-4E1E-91F4-22754FFFE3CC}" name="HP2" dataDxfId="2">
+    <tableColumn id="14" xr3:uid="{6E9D2E4F-4D5A-4E1E-91F4-22754FFFE3CC}" name="HP2" dataDxfId="3">
       <calculatedColumnFormula>SUM(Table8[[#This Row],[HP]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[HP]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{BCBD232D-B15D-4401-9CF2-DC0F3D6CC7D1}" name="Ability" dataDxfId="1">
+    <tableColumn id="15" xr3:uid="{BCBD232D-B15D-4401-9CF2-DC0F3D6CC7D1}" name="Ability" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Ability])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{AFEF4760-EB7A-4908-B1B6-2F830AC5F848}" name="Power/Cost2" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{AFEF4760-EB7A-4908-B1B6-2F830AC5F848}" name="Power/Cost2" dataDxfId="1">
       <calculatedColumnFormula>(Table8[[#This Row],[PP2]]+(Table8[[#This Row],[HP2]]/2)+IF(Table8[[#This Row],[Ability 1]]=0,0,1)+IF(Table8[[#This Row],[Ability 2]]=0,0,1))/(Table8[[#This Row],[Cost]]+1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3075,19 +3144,19 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7A4F3B76-8375-4FD9-8128-9BF9E8EECA3E}" name="Table2" displayName="Table2" ref="A1:G49" totalsRowShown="0" headerRowDxfId="114" dataDxfId="113">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7A4F3B76-8375-4FD9-8128-9BF9E8EECA3E}" name="Table2" displayName="Table2" ref="A1:G49" totalsRowShown="0" headerRowDxfId="115" dataDxfId="114">
   <autoFilter ref="A1:G49" xr:uid="{7A4F3B76-8375-4FD9-8128-9BF9E8EECA3E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G52">
     <sortCondition ref="B1:B52"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{44860EA4-FD5F-4598-AEEF-F7BFC26B7043}" name="Name" dataDxfId="112"/>
-    <tableColumn id="2" xr3:uid="{1D3C02DC-E11C-4FFB-A25C-614675F78ABA}" name="Type" dataDxfId="111"/>
-    <tableColumn id="3" xr3:uid="{E017E39D-29F1-4E55-98B2-8FC221A535CB}" name="Cost" dataDxfId="110"/>
-    <tableColumn id="4" xr3:uid="{0C4B96A8-AEC8-4A0E-8BE8-D7CB34749D2F}" name="PP" dataDxfId="109"/>
-    <tableColumn id="6" xr3:uid="{C3850DEF-7805-4A9E-9633-EEEB17887BC8}" name="Abiliity" dataDxfId="108"/>
-    <tableColumn id="7" xr3:uid="{1ED89F1A-CDCF-47EE-9E26-6872FAA8597A}" name="Ability no" dataDxfId="107"/>
-    <tableColumn id="9" xr3:uid="{0958D538-E9B7-4AEC-AF18-35CC9DE38D59}" name="Sample Bot" dataDxfId="106">
+    <tableColumn id="1" xr3:uid="{44860EA4-FD5F-4598-AEEF-F7BFC26B7043}" name="Name" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{1D3C02DC-E11C-4FFB-A25C-614675F78ABA}" name="Type" dataDxfId="112"/>
+    <tableColumn id="3" xr3:uid="{E017E39D-29F1-4E55-98B2-8FC221A535CB}" name="Cost" dataDxfId="111"/>
+    <tableColumn id="4" xr3:uid="{0C4B96A8-AEC8-4A0E-8BE8-D7CB34749D2F}" name="PP" dataDxfId="110"/>
+    <tableColumn id="6" xr3:uid="{C3850DEF-7805-4A9E-9633-EEEB17887BC8}" name="Abiliity" dataDxfId="109"/>
+    <tableColumn id="7" xr3:uid="{1ED89F1A-CDCF-47EE-9E26-6872FAA8597A}" name="Ability no" dataDxfId="108"/>
+    <tableColumn id="9" xr3:uid="{0958D538-E9B7-4AEC-AF18-35CC9DE38D59}" name="Sample Bot" dataDxfId="107">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3096,19 +3165,19 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C36EF94-5A06-4496-A2EF-5A49AF4820A5}" name="Table1" displayName="Table1" ref="A1:G49" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C36EF94-5A06-4496-A2EF-5A49AF4820A5}" name="Table1" displayName="Table1" ref="A1:G49" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93">
   <autoFilter ref="A1:G49" xr:uid="{7C36EF94-5A06-4496-A2EF-5A49AF4820A5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G49">
     <sortCondition ref="B1:B49"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{61B2C0C4-A5E9-43E9-9491-4023700908E2}" name="Name" dataDxfId="91"/>
-    <tableColumn id="2" xr3:uid="{0043821A-9ACC-4B46-A77D-FA6E1160DB7D}" name="Type" dataDxfId="90"/>
-    <tableColumn id="3" xr3:uid="{811FF43C-AC71-46BA-860D-A5DF9BCD7BD9}" name="Cost" dataDxfId="89"/>
-    <tableColumn id="4" xr3:uid="{3CD0D579-A4FE-4F55-8116-F9E3E83087DE}" name="HP" dataDxfId="88"/>
-    <tableColumn id="5" xr3:uid="{69B3E0C2-96A3-48E0-9C7B-7BA5DA160A3F}" name="Ability" dataDxfId="87"/>
-    <tableColumn id="6" xr3:uid="{E504C788-FE7C-4DDA-A5B2-EFCEA25ABA78}" name="Ability No" dataDxfId="86"/>
-    <tableColumn id="8" xr3:uid="{15023E0C-2733-4E6F-B7AD-8AF7DAD2C257}" name="Sample Bot" dataDxfId="85">
+    <tableColumn id="1" xr3:uid="{61B2C0C4-A5E9-43E9-9491-4023700908E2}" name="Name" dataDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{0043821A-9ACC-4B46-A77D-FA6E1160DB7D}" name="Type" dataDxfId="91"/>
+    <tableColumn id="3" xr3:uid="{811FF43C-AC71-46BA-860D-A5DF9BCD7BD9}" name="Cost" dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{3CD0D579-A4FE-4F55-8116-F9E3E83087DE}" name="HP" dataDxfId="89"/>
+    <tableColumn id="5" xr3:uid="{69B3E0C2-96A3-48E0-9C7B-7BA5DA160A3F}" name="Ability" dataDxfId="88"/>
+    <tableColumn id="6" xr3:uid="{E504C788-FE7C-4DDA-A5B2-EFCEA25ABA78}" name="Ability No" dataDxfId="87"/>
+    <tableColumn id="8" xr3:uid="{15023E0C-2733-4E6F-B7AD-8AF7DAD2C257}" name="Sample Bot" dataDxfId="86">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3117,25 +3186,25 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{AC6516ED-FA98-4523-83EE-69A55ECFF39F}" name="Variety" displayName="Variety" ref="A4:G10" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{AC6516ED-FA98-4523-83EE-69A55ECFF39F}" name="Variety" displayName="Variety" ref="A4:G10" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A4:G10" xr:uid="{AC6516ED-FA98-4523-83EE-69A55ECFF39F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:G10">
     <sortCondition ref="A4:A10"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0D866C81-1CAB-4FD7-97E5-8378FE482ECB}" name="Type" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{9A9DEA20-92D8-4011-950B-D6302196503D}" name="Ideal" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{1C762ECE-0C98-4920-B0E4-55A7A19F83FE}" name="Actual" dataDxfId="56">
+    <tableColumn id="1" xr3:uid="{0D866C81-1CAB-4FD7-97E5-8378FE482ECB}" name="Type" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{9A9DEA20-92D8-4011-950B-D6302196503D}" name="Ideal" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{1C762ECE-0C98-4920-B0E4-55A7A19F83FE}" name="Actual" dataDxfId="57">
       <calculatedColumnFormula>COUNTIF(Table1[Type],Variety[[#This Row],[Type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0C8BE51C-0A54-4ED3-B98C-1D7DB953F369}" name="Difference" dataDxfId="55">
+    <tableColumn id="4" xr3:uid="{0C8BE51C-0A54-4ED3-B98C-1D7DB953F369}" name="Difference" dataDxfId="56">
       <calculatedColumnFormula>C5-B5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{3AED6875-DAF4-4906-BE77-76EDD3B57540}" name="Ideal2" dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{2038FDEC-12A5-484F-BDCE-984800935EE8}" name="Actual3" dataDxfId="53">
+    <tableColumn id="5" xr3:uid="{3AED6875-DAF4-4906-BE77-76EDD3B57540}" name="Ideal2" dataDxfId="55"/>
+    <tableColumn id="6" xr3:uid="{2038FDEC-12A5-484F-BDCE-984800935EE8}" name="Actual3" dataDxfId="54">
       <calculatedColumnFormula>COUNTIF(Table2[Type],Variety[[#This Row],[Type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F7D4ECF7-C059-4A05-99E4-7061721663F5}" name="Difference4" dataDxfId="52">
+    <tableColumn id="7" xr3:uid="{F7D4ECF7-C059-4A05-99E4-7061721663F5}" name="Difference4" dataDxfId="53">
       <calculatedColumnFormula>F5-E5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3144,32 +3213,32 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{0A7EB303-0E7F-45E7-8409-4BDD8FBA1748}" name="Stats" displayName="Stats" ref="A14:J20" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{0A7EB303-0E7F-45E7-8409-4BDD8FBA1748}" name="Stats" displayName="Stats" ref="A14:J20" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="A14:J20" xr:uid="{0A7EB303-0E7F-45E7-8409-4BDD8FBA1748}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:J20">
     <sortCondition ref="A14:A20"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{7EB7684E-4D07-449A-BFD3-43839697E526}" name="Type" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{75578D46-0A1F-4356-BCA2-A452E28A1417}" name="Ideal" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{B17B7A7F-D00A-4E52-B2CF-783A8BDD18B4}" name="Actual" dataDxfId="47">
+    <tableColumn id="1" xr3:uid="{7EB7684E-4D07-449A-BFD3-43839697E526}" name="Type" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{75578D46-0A1F-4356-BCA2-A452E28A1417}" name="Ideal" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{B17B7A7F-D00A-4E52-B2CF-783A8BDD18B4}" name="Actual" dataDxfId="48">
       <calculatedColumnFormula>SUMIF(Table1[Type],Stats[[#This Row],[Type]],Table1[HP])/COUNTIF(Table1[Type],Stats[[#This Row],[Type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A3CF985F-4F0F-467E-93FF-CB89776629BB}" name="Difference" dataDxfId="46">
+    <tableColumn id="4" xr3:uid="{A3CF985F-4F0F-467E-93FF-CB89776629BB}" name="Difference" dataDxfId="47">
       <calculatedColumnFormula>C15-B15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8BFB7AA2-1B75-4F79-966A-74B6F8ED5B7F}" name="Ideal2" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{BE17EF79-FC56-4637-9C8B-66F29560F811}" name="Actual3" dataDxfId="44">
+    <tableColumn id="5" xr3:uid="{8BFB7AA2-1B75-4F79-966A-74B6F8ED5B7F}" name="Ideal2" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{BE17EF79-FC56-4637-9C8B-66F29560F811}" name="Actual3" dataDxfId="45">
       <calculatedColumnFormula array="1">SUMIF(Table2[Type],Stats[[#This Row],[Type]],Table2[PP])/COUNTIF(Table2[Type],Stats[[#This Row],[Type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{583ABFEB-99E8-4030-BFD2-685DD430FA80}" name="Difference4" dataDxfId="43">
+    <tableColumn id="7" xr3:uid="{583ABFEB-99E8-4030-BFD2-685DD430FA80}" name="Difference4" dataDxfId="44">
       <calculatedColumnFormula>F15-E15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B3A60430-2211-48DF-B47C-68AE8FB6A2BB}" name="Ideal5" dataDxfId="42"/>
-    <tableColumn id="9" xr3:uid="{E6BC29A1-559E-44E9-A302-CE348EC0B5D9}" name="Actual6" dataDxfId="41">
+    <tableColumn id="8" xr3:uid="{B3A60430-2211-48DF-B47C-68AE8FB6A2BB}" name="Ideal5" dataDxfId="43"/>
+    <tableColumn id="9" xr3:uid="{E6BC29A1-559E-44E9-A302-CE348EC0B5D9}" name="Actual6" dataDxfId="42">
       <calculatedColumnFormula>(SUMIF(Table1[Type],Stats[[#This Row],[Type]],Table1[Ability No])+SUMIF(Table2[Type],Stats[[#This Row],[Type]],Table2[Ability no]))/(COUNTIF(Table1[Type],Stats[[#This Row],[Type]])+COUNTIF(Table2[Type],Stats[[#This Row],[Type]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5E66CDD0-39AD-4632-9676-0BF8F6414C7E}" name="Difference7" dataDxfId="40">
+    <tableColumn id="10" xr3:uid="{5E66CDD0-39AD-4632-9676-0BF8F6414C7E}" name="Difference7" dataDxfId="41">
       <calculatedColumnFormula>I15-H15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3178,39 +3247,39 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{D9B208C6-E117-47B0-B9C7-9A034FB99F5B}" name="Cost_Stat" displayName="Cost_Stat" ref="A24:M30" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{D9B208C6-E117-47B0-B9C7-9A034FB99F5B}" name="Cost_Stat" displayName="Cost_Stat" ref="A24:M30" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A24:M30" xr:uid="{D9B208C6-E117-47B0-B9C7-9A034FB99F5B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:M30">
     <sortCondition ref="A24:A30"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{F7B32CDF-9BB4-47AF-BE3F-842F7D6EF736}" name="Type" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{E517E5F7-276F-406B-A78C-73C12B03024A}" name="Ideal" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{54CFC0BE-CB89-4B6F-9EA5-3D4D0425EF87}" name="Actual" dataDxfId="35">
+    <tableColumn id="1" xr3:uid="{F7B32CDF-9BB4-47AF-BE3F-842F7D6EF736}" name="Type" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{E517E5F7-276F-406B-A78C-73C12B03024A}" name="Ideal" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{54CFC0BE-CB89-4B6F-9EA5-3D4D0425EF87}" name="Actual" dataDxfId="36">
       <calculatedColumnFormula>SUMIF(Table1[Type],Cost_Stat[[#This Row],[Type]],Table1[HP])/SUMIF(Table1[Type],Cost_Stat[[#This Row],[Type]],Table1[Cost])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{485B5A87-DD44-4B1F-95C2-F593EAB7581E}" name="Difference" dataDxfId="34">
+    <tableColumn id="4" xr3:uid="{485B5A87-DD44-4B1F-95C2-F593EAB7581E}" name="Difference" dataDxfId="35">
       <calculatedColumnFormula>C25-B25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{0AB55B04-7DB1-4B3B-95A0-41BE01235610}" name="Ideal2" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{EBE0B5B1-010C-4B8E-BF94-291D680A295E}" name="Actual3" dataDxfId="32">
+    <tableColumn id="5" xr3:uid="{0AB55B04-7DB1-4B3B-95A0-41BE01235610}" name="Ideal2" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{EBE0B5B1-010C-4B8E-BF94-291D680A295E}" name="Actual3" dataDxfId="33">
       <calculatedColumnFormula>SUMIF(Table2[Type],Cost_Stat[[#This Row],[Type]],Table2[PP])/SUMIF(Table2[Type],Cost_Stat[[#This Row],[Type]],Table2[Cost])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{DF4CF3C4-B12B-46B7-BC59-E5351C495BC1}" name="Difference4" dataDxfId="31">
+    <tableColumn id="7" xr3:uid="{DF4CF3C4-B12B-46B7-BC59-E5351C495BC1}" name="Difference4" dataDxfId="32">
       <calculatedColumnFormula>F25-E25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{466E32FE-7121-4644-899F-C08F4CE38771}" name="Ideal5" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{FF597456-2300-4BC6-8B64-D1A298F13E5A}" name="Actual6" dataDxfId="29">
+    <tableColumn id="8" xr3:uid="{466E32FE-7121-4644-899F-C08F4CE38771}" name="Ideal5" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{FF597456-2300-4BC6-8B64-D1A298F13E5A}" name="Actual6" dataDxfId="30">
       <calculatedColumnFormula>(SUMIF(Table1[Type],Cost_Stat[[#This Row],[Type]],Table1[Ability No])+SUMIF(Table2[Type],Cost_Stat[[#This Row],[Type]],Table2[Ability no]))/(SUMIFS(Table1[Cost],Table1[Type],Cost_Stat[[#This Row],[Type]],Table1[Ability No],1)+SUMIFS(Table2[Cost],Table2[Type],Cost_Stat[[#This Row],[Type]],Table2[Ability no],1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{FB0F2832-C6B6-4855-8222-A7A9323ACFC9}" name="Difference7" dataDxfId="28">
+    <tableColumn id="10" xr3:uid="{FB0F2832-C6B6-4855-8222-A7A9323ACFC9}" name="Difference7" dataDxfId="29">
       <calculatedColumnFormula>I25-H25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{73909C54-2246-4ED8-B808-E4BE1DD4A485}" name="Ideal8" dataDxfId="27"/>
-    <tableColumn id="12" xr3:uid="{2B1962BE-7805-4FFA-8D3C-E67730E4E5EA}" name="Actual9" dataDxfId="26">
+    <tableColumn id="11" xr3:uid="{73909C54-2246-4ED8-B808-E4BE1DD4A485}" name="Ideal8" dataDxfId="28"/>
+    <tableColumn id="12" xr3:uid="{2B1962BE-7805-4FFA-8D3C-E67730E4E5EA}" name="Actual9" dataDxfId="27">
       <calculatedColumnFormula>(SUMIF(Table1[Type],Cost_Stat[[#This Row],[Type]],Table1[Cost])+SUMIF(Table2[Type],Cost_Stat[[#This Row],[Type]],Table2[Cost]))/(COUNTIF(Table1[Type],Cost_Stat[[#This Row],[Type]])+COUNTIF(Table2[Type],Cost_Stat[[#This Row],[Type]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{05006522-125E-42FB-A202-48124F65E1AF}" name="Difference10" dataDxfId="25">
+    <tableColumn id="13" xr3:uid="{05006522-125E-42FB-A202-48124F65E1AF}" name="Difference10" dataDxfId="26">
       <calculatedColumnFormula>L25-K25</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3219,17 +3288,17 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{CFB70296-300F-41E9-B29C-A15C0D2E492E}" name="Table15" displayName="Table15" ref="L14:O20" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{CFB70296-300F-41E9-B29C-A15C0D2E492E}" name="Table15" displayName="Table15" ref="L14:O20" totalsRowShown="0" headerRowDxfId="25" tableBorderDxfId="24">
   <autoFilter ref="L14:O20" xr:uid="{CFB70296-300F-41E9-B29C-A15C0D2E492E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{67B9F3DD-84E5-4E12-9557-0E15E2E8CD01}" name="Type" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{882509E9-98E0-4845-9863-913DA546EA5B}" name="Cost" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{67B9F3DD-84E5-4E12-9557-0E15E2E8CD01}" name="Type" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{882509E9-98E0-4845-9863-913DA546EA5B}" name="Cost" dataDxfId="22">
       <calculatedColumnFormula>ROUND(2*SUMIF(Cost_Stat[Type],Table15[[#This Row],[Type]],Cost_Stat[Actual9]),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8E6F0F0A-DEBA-4962-9C42-B7696451440A}" name="HP" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{8E6F0F0A-DEBA-4962-9C42-B7696451440A}" name="HP" dataDxfId="21">
       <calculatedColumnFormula>Table15[[#This Row],[Cost]]*SUMIF(Cost_Stat[Type],Table15[[#This Row],[Type]],Cost_Stat[Actual])/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8646B895-6FEE-4C10-AE30-8852BA384EB5}" name="PP" dataDxfId="19">
+    <tableColumn id="8" xr3:uid="{8646B895-6FEE-4C10-AE30-8852BA384EB5}" name="PP" dataDxfId="20">
       <calculatedColumnFormula>Table15[[#This Row],[Cost]]*SUMIF(Cost_Stat[Type],Table15[[#This Row],[Type]],Cost_Stat[Actual3])/2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3238,18 +3307,18 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BD6F9D4F-C6DA-4DA9-9AF2-B383883F498D}" name="Table3" displayName="Table3" ref="A1:F23" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BD6F9D4F-C6DA-4DA9-9AF2-B383883F498D}" name="Table3" displayName="Table3" ref="A1:F23" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:F23" xr:uid="{BD6F9D4F-C6DA-4DA9-9AF2-B383883F498D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E23">
     <sortCondition descending="1" ref="E1:E23"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{98031720-D200-46F3-9ACA-C1755FECC5FB}" name="Name" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{EF26975E-EC1C-434E-9124-8EA3E2771B2B}" name="Cost" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{B5C3D5E2-952F-4B3E-9501-9A5F8E406832}" name="HP" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{91393694-5AF1-4A22-906A-4DDEB27DF551}" name="PP" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{25DD586E-BA8D-4FFE-A5E1-28663B66B645}" name="Ability" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{EF00229C-6DD0-499F-B5E4-58AB07CFF4F4}" name="Ability No" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{98031720-D200-46F3-9ACA-C1755FECC5FB}" name="Name" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{EF26975E-EC1C-434E-9124-8EA3E2771B2B}" name="Cost" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{B5C3D5E2-952F-4B3E-9501-9A5F8E406832}" name="HP" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{91393694-5AF1-4A22-906A-4DDEB27DF551}" name="PP" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{25DD586E-BA8D-4FFE-A5E1-28663B66B645}" name="Ability" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{EF00229C-6DD0-499F-B5E4-58AB07CFF4F4}" name="Ability No" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3552,10 +3621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798D3000-7536-4EA3-B16D-80887633F251}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection sqref="A1:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3564,7 +3633,7 @@
     <col min="3" max="3" width="65.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -3572,281 +3641,449 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>207</v>
       </c>
       <c r="B2" t="s">
         <v>78</v>
       </c>
-      <c r="C2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="str">
+        <f>"+2 HP each time an opponent builds a bot"</f>
+        <v>+2 HP each time an opponent builds a bot</v>
+      </c>
+      <c r="E2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
         <v>78</v>
       </c>
-      <c r="C3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f>"+1 PP whenever opponent bot gains PP"</f>
+        <v>+1 PP whenever opponent bot gains PP</v>
+      </c>
+      <c r="E3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>210</v>
       </c>
       <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="str">
+        <f>"-1 PP to draw a card once per turn"</f>
+        <v>-1 PP to draw a card once per turn</v>
+      </c>
+      <c r="E5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="str">
+        <f>"+2 HP each time you draw a card"</f>
+        <v>+2 HP each time you draw a card</v>
+      </c>
+      <c r="E6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="str">
-        <f>"+10 HP per turn for each upgrade on this bot"</f>
-        <v>+10 HP per turn for each upgrade on this bot</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="str">
-        <f>"-1 cost to upgrades"</f>
-        <v>-1 cost to upgrades</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>207</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="str">
+      <c r="D7" t="str">
         <f>"+1 PP per turn for each upgrade on this bot"</f>
         <v>+1 PP per turn for each upgrade on this bot</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E7" t="s">
         <v>208</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="str">
-        <f>"+2 PP when an ally bot is upgraded"</f>
-        <v>+2 PP when an ally bot is upgraded</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>209</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="str">
-        <f>"+20 HP when an ally bot is upgraded"</f>
-        <v>+20 HP when an ally bot is upgraded</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="str">
+        <f>"+1 dmg dealt for each upgrade on this bot"</f>
+        <v>+1 dmg dealt for each upgrade on this bot</v>
+      </c>
+      <c r="E8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="str">
+        <f>"-1 PP cost to upgrades"</f>
+        <v>-1 PP cost to upgrades</v>
+      </c>
+      <c r="E9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="str">
+        <f>"+2 HP when an ally bot is upgraded"</f>
+        <v>+2 HP when an ally bot is upgraded</v>
+      </c>
+      <c r="E10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="str">
-        <f>"+2 PP each time you mine a new resource"</f>
-        <v>+2 PP each time you mine a new resource</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>202</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>216</v>
+      </c>
+      <c r="E11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="str">
+      <c r="D12" t="str">
+        <f>"+2 PP each time an enemy bot is destroyed"</f>
+        <v>+2 PP each time an enemy bot is destroyed</v>
+      </c>
+      <c r="E12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="str">
+        <f>"+2 HP each time you mine a new resource"</f>
+        <v>+2 HP each time you mine a new resource</v>
+      </c>
+      <c r="E13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>218</v>
+      </c>
+      <c r="E14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="str">
         <f>"-1 PP cost the first time you mine a new resource each turn"</f>
         <v>-1 PP cost the first time you mine a new resource each turn</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="E15" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>219</v>
+      </c>
+      <c r="B16" t="s">
         <v>45</v>
       </c>
-      <c r="C13" t="str">
-        <f>"-1 PP cost to move this bot"</f>
-        <v>-1 PP cost to move this bot</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>131</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D16" t="str">
+        <f>"-1 PP to power a bot"</f>
+        <v>-1 PP to power a bot</v>
+      </c>
+      <c r="E16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="C14" t="str">
-        <f>"+2 PP each time a bot moves"</f>
-        <v>+2 PP each time a bot moves</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>200</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="59" t="str">
+      <c r="D17" s="52" t="str">
         <f>"+1 PP from each non-adjacent Weather Event resource"</f>
         <v>+1 PP from each non-adjacent Weather Event resource</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="E17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" t="str">
+        <f>"-1 PP cost to move a bot the first time each turn"</f>
+        <v>-1 PP cost to move a bot the first time each turn</v>
+      </c>
+      <c r="E18" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="str">
+        <f>"+2 HP each time a bot moves"</f>
+        <v>+2 HP each time a bot moves</v>
+      </c>
+      <c r="E19" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>205</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="str">
+        <f>"+2 HP each time a bot moves"</f>
+        <v>+2 HP each time a bot moves</v>
+      </c>
+      <c r="E20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>196</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B21" t="s">
         <v>16</v>
       </c>
-      <c r="C16" t="str">
-        <f>"+10 hp each turn for each active friendly bot"</f>
-        <v>+10 hp each turn for each active friendly bot</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D21" t="str">
+        <f>"+2 PP each time a friendly bot is destroyed"</f>
+        <v>+2 PP each time a friendly bot is destroyed</v>
+      </c>
+      <c r="E21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>96</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B22" t="s">
         <v>16</v>
       </c>
-      <c r="C17" t="str">
-        <f>"+1 pp each turn for each active friendly bot"</f>
-        <v>+1 pp each turn for each active friendly bot</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D22" t="str">
+        <f>"+1 PP each turn for each active friendly bot"</f>
+        <v>+1 PP each turn for each active friendly bot</v>
+      </c>
+      <c r="E22" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>90</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B23" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="str">
+      <c r="D23" t="str">
         <f>"-1 PP cost for new bots"</f>
         <v>-1 PP cost for new bots</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="E23" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>197</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B24" t="s">
         <v>16</v>
       </c>
-      <c r="C19" t="str">
-        <f>"+20 HP each time a new bot is built"</f>
-        <v>+20 HP each time a new bot is built</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>198</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" t="str">
-        <f>"+2 PP each time a new bot is built"</f>
-        <v>+2 PP each time a new bot is built</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>206</v>
-      </c>
-      <c r="B21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" t="str">
-        <f>"-1 PP cost to the bots in your hand each time this bot regains HP"</f>
-        <v>-1 PP cost to the bots in your hand each time this bot regains HP</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="D24" t="str">
+        <f>"+2 HP each time a new bot is built"</f>
+        <v>+2 HP each time a new bot is built</v>
+      </c>
+      <c r="E24" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>44</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>22</v>
       </c>
-      <c r="C22" t="str">
-        <f>"-10 dmg to each attack"</f>
-        <v>-10 dmg to each attack</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>91</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="D25" t="str">
+        <f>"-1 dmg to each attack against this bot"</f>
+        <v>-1 dmg to each attack against this bot</v>
+      </c>
+      <c r="E25" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>221</v>
+      </c>
+      <c r="B26" t="s">
         <v>22</v>
       </c>
-      <c r="C23" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>210</v>
-      </c>
-      <c r="B24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" t="str">
-        <f>"+20 HP each time a bot moves"</f>
-        <v>+20 HP each time a bot moves</v>
+      <c r="D26" t="str">
+        <f>"+2 PP each time you play a mechanic card"</f>
+        <v>+2 PP each time you play a mechanic card</v>
+      </c>
+      <c r="E26" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>222</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>223</v>
+      </c>
+      <c r="E27" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>224</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
+        <v>225</v>
+      </c>
+      <c r="E28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>226</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>227</v>
+      </c>
+      <c r="E29" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>228</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>229</v>
+      </c>
+      <c r="E30" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:E30">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -4060,7 +4297,7 @@
       <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="59" t="str">
+      <c r="C17" s="52" t="str">
         <f>"+1 PP from each non-adjacent Weather Event resource"</f>
         <v>+1 PP from each non-adjacent Weather Event resource</v>
       </c>
@@ -4156,7 +4393,7 @@
       </c>
       <c r="G3" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G3" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>SYNAnacht</v>
+        <v>SYNAfel</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -4181,7 +4418,7 @@
       </c>
       <c r="G4" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G4" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>LUNAnyx</v>
+        <v>LUNAfel</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -4206,7 +4443,7 @@
       </c>
       <c r="G5" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G5" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>UMBRAklum</v>
+        <v>UMBRAfel</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -4231,7 +4468,7 @@
       </c>
       <c r="G6" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G6" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>KLEPTOply</v>
+        <v>KLEPTOmyth</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -4256,7 +4493,7 @@
       </c>
       <c r="G7" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G7" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>CORVAnyx</v>
+        <v>CORVAfel</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -4281,7 +4518,7 @@
       </c>
       <c r="G8" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G8" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>HYPNOrect</v>
+        <v>HYPNOfel</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -4306,7 +4543,7 @@
       </c>
       <c r="G9" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G9" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>DEXTRAklum</v>
+        <v>DEXTRAmyth</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -4357,7 +4594,7 @@
       </c>
       <c r="G11" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G11" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>NUCLEtheum</v>
+        <v>NUCLElium</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -4382,7 +4619,7 @@
       </c>
       <c r="G12" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G12" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>RADIzone</v>
+        <v>RADIline</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -4407,7 +4644,7 @@
       </c>
       <c r="G13" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G13" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>NEOtheum</v>
+        <v>NEOneon</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -4430,7 +4667,7 @@
       </c>
       <c r="G14" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G14" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>PLUTOlium</v>
+        <v>PLUTOneon</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -4455,7 +4692,7 @@
       </c>
       <c r="G15" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G15" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>URAtheum</v>
+        <v>URAnite</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -4480,7 +4717,7 @@
       </c>
       <c r="G16" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>FERRUlium</v>
+        <v>FERRUbium</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4505,7 +4742,7 @@
       </c>
       <c r="G17" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G17" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>COLAbium</v>
+        <v>COLAtheum</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4528,7 +4765,7 @@
       </c>
       <c r="G18" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>ANTHRAkar</v>
+        <v>ANTHRAdon</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4551,7 +4788,7 @@
       </c>
       <c r="G19" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>CHARIbar</v>
+        <v>CHARIkar</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4576,7 +4813,7 @@
       </c>
       <c r="G20" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>ATMOton</v>
+        <v>ATMOdon</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4601,7 +4838,7 @@
       </c>
       <c r="G21" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>EXPLOdon</v>
+        <v>EXPLOgul</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4624,7 +4861,7 @@
       </c>
       <c r="G22" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>OLEUgul</v>
+        <v>OLEUkar</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4649,7 +4886,7 @@
       </c>
       <c r="G23" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>PYROdon</v>
+        <v>PYROgul</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4674,7 +4911,7 @@
       </c>
       <c r="G24" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G24" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>THURMAkar</v>
+        <v>THURMAtus</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4697,7 +4934,7 @@
       </c>
       <c r="G25" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G25" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>FIRAbar</v>
+        <v>FIRAgon</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4720,7 +4957,7 @@
       </c>
       <c r="G26" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G26" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>GEOviz</v>
+        <v>GEOgar</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4743,7 +4980,7 @@
       </c>
       <c r="G27" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G27" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>VAPOtalus</v>
+        <v>VAPOform</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4768,7 +5005,7 @@
       </c>
       <c r="G28" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G28" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>AEROmorph</v>
+        <v>AEROtine</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4791,7 +5028,7 @@
       </c>
       <c r="G29" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G29" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>AQUAviz</v>
+        <v>AQUAform</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4816,7 +5053,7 @@
       </c>
       <c r="G30" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G30" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>SOLAmorph</v>
+        <v>SOLAgar</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4841,7 +5078,7 @@
       </c>
       <c r="G31" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G31" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>VENTRAnax</v>
+        <v>VENTRAform</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4866,7 +5103,7 @@
       </c>
       <c r="G32" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G32" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>HELIOmant</v>
+        <v>HELIOnax</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4889,7 +5126,7 @@
       </c>
       <c r="G33" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G33" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>HYDROgar</v>
+        <v>HYDROnax</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4914,7 +5151,7 @@
       </c>
       <c r="G34" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G34" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>CARNIlophus</v>
+        <v>CARNIsuarus</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4937,7 +5174,7 @@
       </c>
       <c r="G35" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G35" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>HERBAphyte</v>
+        <v>HERBActos</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4985,7 +5222,7 @@
       </c>
       <c r="G37" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G37" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>FAUNAvore</v>
+        <v>FAUNAling</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -5010,7 +5247,7 @@
       </c>
       <c r="G38" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G38" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>PREDAvore</v>
+        <v>PREDActos</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -5035,7 +5272,7 @@
       </c>
       <c r="G39" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G39" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>FOLIsuarus</v>
+        <v>FOLIctos</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -5060,7 +5297,7 @@
       </c>
       <c r="G40" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G40" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>CANOling</v>
+        <v>CANOsuarus</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -5085,7 +5322,7 @@
       </c>
       <c r="G41" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G41" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>LEPHAlophus</v>
+        <v>LEPHAphyte</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -5108,7 +5345,7 @@
       </c>
       <c r="G42" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G42" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>MEGAcell</v>
+        <v>MEGAdome</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -5131,7 +5368,7 @@
       </c>
       <c r="G43" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G43" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>GIGAlite</v>
+        <v>GIGAhull</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -5156,7 +5393,7 @@
       </c>
       <c r="G44" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G44" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>SUPRAbyte</v>
+        <v>SUPRAshell</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -5181,7 +5418,7 @@
       </c>
       <c r="G45" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G45" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>TERAbyte</v>
+        <v>TERAhull</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -5229,7 +5466,7 @@
       </c>
       <c r="G47" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G47" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>TURBOshell</v>
+        <v>TURBOhull</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -5252,7 +5489,7 @@
       </c>
       <c r="G48" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G48" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>DYNAstega</v>
+        <v>DYNAlite</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -5277,7 +5514,7 @@
       </c>
       <c r="G49" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G49" ca="1">_xlfn.CONCAT(UPPER(Table2[[#This Row],[Name]]),INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table2[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table2[[#This Row],[Type]])+1))))</f>
-        <v>CYCLOhull</v>
+        <v>CYCLOshell</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -5379,78 +5616,78 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F49">
-    <cfRule type="cellIs" dxfId="138" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="13" operator="equal">
       <formula>"Preserve"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="14" operator="equal">
       <formula>"Cultivate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="15" operator="equal">
       <formula>"Convert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="16" operator="equal">
       <formula>"Consume"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="17" operator="equal">
       <formula>"Augment"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="18" operator="equal">
       <formula>"Acquire"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="19">
+    <cfRule type="expression" dxfId="133" priority="19">
       <formula>$B1="Acquire"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="20">
+    <cfRule type="expression" dxfId="132" priority="20">
       <formula>$B1="Augment"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="21">
+    <cfRule type="expression" dxfId="131" priority="21">
       <formula>$B1="Consume"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="22">
+    <cfRule type="expression" dxfId="130" priority="22">
       <formula>$B1="Convert"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="23">
+    <cfRule type="expression" dxfId="129" priority="23">
       <formula>$B1="Cultivate"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="24">
+    <cfRule type="expression" dxfId="128" priority="24">
       <formula>$B1="Preserve"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G49">
-    <cfRule type="cellIs" dxfId="126" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="1" operator="equal">
       <formula>"Preserve"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="2" operator="equal">
       <formula>"Cultivate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="3" operator="equal">
       <formula>"Convert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="4" operator="equal">
       <formula>"Consume"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="5" operator="equal">
       <formula>"Augment"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="6" operator="equal">
       <formula>"Acquire"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="7">
+    <cfRule type="expression" dxfId="121" priority="7">
       <formula>$B1="Acquire"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="8">
+    <cfRule type="expression" dxfId="120" priority="8">
       <formula>$B1="Augment"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="9">
+    <cfRule type="expression" dxfId="119" priority="9">
       <formula>$B1="Consume"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="10">
+    <cfRule type="expression" dxfId="118" priority="10">
       <formula>$B1="Convert"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="11">
+    <cfRule type="expression" dxfId="117" priority="11">
       <formula>$B1="Cultivate"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="12">
+    <cfRule type="expression" dxfId="116" priority="12">
       <formula>$B1="Preserve"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5480,7 +5717,7 @@
     <col min="8" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -5523,7 +5760,7 @@
       </c>
       <c r="G2" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G2" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>CorvaRECT</v>
+        <v>DextraRECT</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -5571,7 +5808,7 @@
       </c>
       <c r="G4" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G4" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>KleptoNACHT</v>
+        <v>LunaNACHT</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -5619,7 +5856,7 @@
       </c>
       <c r="G6" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G6" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>KleptoKLUM</v>
+        <v>HypnoKLUM</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -5642,7 +5879,7 @@
       </c>
       <c r="G7" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G7" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>KleptoFEL</v>
+        <v>HypnoFEL</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -5667,7 +5904,7 @@
       </c>
       <c r="G8" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G8" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>UmbraMYTH</v>
+        <v>SynaMYTH</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -5692,7 +5929,7 @@
       </c>
       <c r="G9" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G9" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>KleptoMORE</v>
+        <v>DextraMORE</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -5715,7 +5952,7 @@
       </c>
       <c r="G10" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G10" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>PlutoNEON</v>
+        <v>FerruNEON</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -5765,7 +6002,7 @@
       </c>
       <c r="G12" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G12" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>ProtoZINE</v>
+        <v>UraZINE</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -5790,7 +6027,7 @@
       </c>
       <c r="G13" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G13" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>NucleLIUM</v>
+        <v>PlutoLIUM</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -5813,7 +6050,7 @@
       </c>
       <c r="G14" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G14" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>FerruNITE</v>
+        <v>PlutoNITE</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -5838,7 +6075,7 @@
       </c>
       <c r="G15" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G15" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>NucleTHEUM</v>
+        <v>ColaTHEUM</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -5861,7 +6098,7 @@
       </c>
       <c r="G16" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>NucleZONE</v>
+        <v>ColaZONE</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -5884,7 +6121,7 @@
       </c>
       <c r="G17" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G17" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>NucleLINE</v>
+        <v>ProtoLINE</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -5907,7 +6144,7 @@
       </c>
       <c r="G18" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>AnthraTON</v>
+        <v>ThurmaTON</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -5930,7 +6167,7 @@
       </c>
       <c r="G19" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>PyroLUS</v>
+        <v>ExploLUS</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -5955,7 +6192,7 @@
       </c>
       <c r="G20" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>ExploDON</v>
+        <v>PyroDON</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -5980,7 +6217,7 @@
       </c>
       <c r="G21" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>ChariKAR</v>
+        <v>ThurmaKAR</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -6005,7 +6242,7 @@
       </c>
       <c r="G22" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>PyroGON</v>
+        <v>ThurmaGON</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -6030,7 +6267,7 @@
       </c>
       <c r="G23" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>AtmoTUS</v>
+        <v>ChariTUS</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -6078,7 +6315,7 @@
       </c>
       <c r="G25" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G25" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>ThurmaGUL</v>
+        <v>PyroGUL</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -6147,7 +6384,7 @@
       </c>
       <c r="G28" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G28" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>HydroMORPH</v>
+        <v>AquaMORPH</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -6197,7 +6434,7 @@
       </c>
       <c r="G30" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G30" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>GeoNAX</v>
+        <v>SolaNAX</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -6220,7 +6457,7 @@
       </c>
       <c r="G31" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G31" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>AquaFORM</v>
+        <v>GeoFORM</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -6245,7 +6482,7 @@
       </c>
       <c r="G32" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G32" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>AeroVIZ</v>
+        <v>HydroVIZ</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -6270,7 +6507,7 @@
       </c>
       <c r="G33" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G33" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>SolaGAR</v>
+        <v>VentraGAR</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -6293,7 +6530,7 @@
       </c>
       <c r="G34" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G34" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>CarniLING</v>
+        <v>FaunaLING</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -6343,7 +6580,7 @@
       </c>
       <c r="G36" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G36" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>CanoPHYTE</v>
+        <v>LephaPHYTE</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -6368,7 +6605,7 @@
       </c>
       <c r="G37" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G37" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>CarniPOD</v>
+        <v>HerbaPOD</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -6391,7 +6628,7 @@
       </c>
       <c r="G38" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G38" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>PredaSUARUS</v>
+        <v>FloraSUARUS</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -6416,7 +6653,7 @@
       </c>
       <c r="G39" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G39" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>FaunaCTOS</v>
+        <v>FoliCTOS</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -6441,7 +6678,7 @@
       </c>
       <c r="G40" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G40" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>FloraLOPHUS</v>
+        <v>LephaLOPHUS</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -6464,7 +6701,7 @@
       </c>
       <c r="G41" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G41" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>PredaCLOR</v>
+        <v>FaunaCLOR</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -6487,7 +6724,7 @@
       </c>
       <c r="G42" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G42" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>CycloBIT</v>
+        <v>DynaBIT</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -6510,7 +6747,7 @@
       </c>
       <c r="G43" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G43" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>TeraBYTE</v>
+        <v>SupraBYTE</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -6535,7 +6772,7 @@
       </c>
       <c r="G44" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G44" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>TeraSTEGA</v>
+        <v>DynaSTEGA</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -6558,7 +6795,7 @@
       </c>
       <c r="G45" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G45" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>CycloCELL</v>
+        <v>UltraCELL</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -6583,7 +6820,7 @@
       </c>
       <c r="G46" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G46" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>CycloLITE</v>
+        <v>SupraLITE</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -6606,7 +6843,7 @@
       </c>
       <c r="G47" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G47" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>DynaSHELL</v>
+        <v>TurboSHELL</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -6631,7 +6868,7 @@
       </c>
       <c r="G48" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G48" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>UltraHULL</v>
+        <v>SupraHULL</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -6656,45 +6893,45 @@
       </c>
       <c r="G49" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="G49" ca="1">_xlfn.CONCAT(INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table1[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table1[[#This Row],[Type]])+1))),UPPER(Table1[[#This Row],[Name]]))</f>
-        <v>UltraDOME</v>
+        <v>TurboDOME</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:G49">
-    <cfRule type="cellIs" dxfId="105" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="13" operator="equal">
       <formula>"Preserve"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="14" operator="equal">
       <formula>"Cultivate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="15" operator="equal">
       <formula>"Convert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="16" operator="equal">
       <formula>"Consume"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="17" operator="equal">
       <formula>"Augment"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="18" operator="equal">
       <formula>"Acquire"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="19">
+    <cfRule type="expression" dxfId="100" priority="19">
       <formula>$B2="Acquire"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="20">
+    <cfRule type="expression" dxfId="99" priority="20">
       <formula>$B2="Augment"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="21">
+    <cfRule type="expression" dxfId="98" priority="21">
       <formula>$B2="Consume"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="22">
+    <cfRule type="expression" dxfId="97" priority="22">
       <formula>$B2="Convert"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="23">
+    <cfRule type="expression" dxfId="96" priority="23">
       <formula>$B2="Cultivate"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="24">
+    <cfRule type="expression" dxfId="95" priority="24">
       <formula>$B2="Preserve"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6732,34 +6969,34 @@
       <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="53" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="57"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="55"/>
       <c r="H2" s="19"/>
-      <c r="I2" s="55" t="s">
+      <c r="I2" s="53" t="s">
         <v>170</v>
       </c>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="57"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="55"/>
       <c r="M2" s="19"/>
     </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="52" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B3" s="57" t="s">
         <v>134</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="52" t="s">
+      <c r="C3" s="58"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="54"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="59"/>
       <c r="H3" s="20"/>
       <c r="I3" s="46" t="s">
         <v>136</v>
@@ -6817,7 +7054,7 @@
       </c>
       <c r="M4" s="13"/>
     </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
         <v>78</v>
       </c>
@@ -6898,7 +7135,7 @@
       </c>
       <c r="M6" s="15"/>
     </row>
-    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
         <v>9</v>
       </c>
@@ -7035,40 +7272,40 @@
     </row>
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="57"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="55"/>
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="52" t="s">
+      <c r="C13" s="58"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="53"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="52" t="s">
+      <c r="F13" s="58"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="I13" s="53"/>
-      <c r="J13" s="54"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="59"/>
       <c r="K13" s="45"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="58"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="56"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
@@ -7451,42 +7688,42 @@
       <c r="J21" s="15"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="53" t="s">
         <v>154</v>
       </c>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="56"/>
-      <c r="I22" s="56"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="57"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="55"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="53"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="52" t="s">
+      <c r="C23" s="58"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="53"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="52" t="s">
+      <c r="F23" s="58"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="I23" s="53"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="52" t="s">
+      <c r="I23" s="58"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="L23" s="53"/>
-      <c r="M23" s="54"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="59"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
@@ -7825,6 +8062,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B22:M22"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="M13:N13"/>
@@ -7833,12 +8076,6 @@
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:G3"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B22:M22"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:G10">
     <cfRule type="dataBar" priority="44">
@@ -7965,62 +8202,62 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A10">
-    <cfRule type="cellIs" dxfId="84" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="36" operator="equal">
       <formula>"Preserve"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="37" operator="equal">
       <formula>"Cultivate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="38" operator="equal">
       <formula>"Convert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="39" operator="equal">
       <formula>"Consume"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="40" operator="equal">
       <formula>"Augment"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="41" operator="equal">
       <formula>"Acquire"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:A20">
-    <cfRule type="cellIs" dxfId="78" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="30" operator="equal">
       <formula>"Preserve"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="31" operator="equal">
       <formula>"Cultivate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="32" operator="equal">
       <formula>"Convert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="33" operator="equal">
       <formula>"Consume"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="34" operator="equal">
       <formula>"Augment"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="35" operator="equal">
       <formula>"Acquire"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:A30">
-    <cfRule type="cellIs" dxfId="72" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="18" operator="equal">
       <formula>"Preserve"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="19" operator="equal">
       <formula>"Cultivate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="20" operator="equal">
       <formula>"Convert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="21" operator="equal">
       <formula>"Consume"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="22" operator="equal">
       <formula>"Augment"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="23" operator="equal">
       <formula>"Acquire"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8095,22 +8332,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15:L20">
-    <cfRule type="cellIs" dxfId="66" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="5" operator="equal">
       <formula>"Preserve"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="6" operator="equal">
       <formula>"Cultivate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="7" operator="equal">
       <formula>"Convert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="8" operator="equal">
       <formula>"Consume"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="9" operator="equal">
       <formula>"Augment"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="10" operator="equal">
       <formula>"Acquire"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8767,67 +9004,67 @@
       </c>
       <c r="B2" t="str" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table8[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table8[[#This Row],[Type]])+1)))</f>
-        <v>Klepto</v>
+        <v>Umbra</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table8[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table8[[#This Row],[Type]])+1)))</f>
-        <v>klum</v>
+        <v>more</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D7" ca="1" si="0">_xlfn.CONCAT(B2,C2)</f>
-        <v>Kleptoklum</v>
+        <v>Umbramore</v>
       </c>
       <c r="E2">
         <f ca="1">SUM(_xlfn.XLOOKUP(Table8[[#This Row],[Generator]],Table2[Name],Table2[Cost]),_xlfn.XLOOKUP(Table8[[#This Row],[Frame]],Table1[Name],Table1[Cost]))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2">
         <f ca="1">_xlfn.XLOOKUP(B2,Table2[Name],Table2[PP])</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <f ca="1">_xlfn.XLOOKUP(C2,Table1[Name],Table1[HP])</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2" t="str">
         <f ca="1">_xlfn.XLOOKUP(B2,Table2[Name],Table2[Abiliity])</f>
-        <v>Reallocate</v>
-      </c>
-      <c r="I2">
+        <v>Flattery</v>
+      </c>
+      <c r="I2" t="str">
         <f ca="1">_xlfn.XLOOKUP(C2,Table1[Name],Table1[Ability])</f>
-        <v>0</v>
+        <v>Flattery</v>
       </c>
       <c r="J2">
         <f ca="1">(Table8[[#This Row],[PP]]+(Table8[[#This Row],[HP]]/2)+IF(Table8[[#This Row],[Ability 1]]=0,0,1)+IF(Table8[[#This Row],[Ability 2]]=0,0,1))/(Table8[[#This Row],[Cost]]+1)</f>
-        <v>2.2000000000000002</v>
+        <v>2.25</v>
       </c>
       <c r="K2" t="str" cm="1">
         <f t="array" aca="1" ref="K2" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>be</v>
+        <v>de</v>
       </c>
       <c r="L2" t="str">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
-        <v>Kleptobeklum</v>
+        <v>Umbrademore</v>
       </c>
       <c r="M2">
         <f ca="1">SUM(Table8[[#This Row],[Cost]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Cost]))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N2">
         <f ca="1">SUM(Table8[[#This Row],[PP]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[PP]))</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O2">
         <f ca="1">SUM(Table8[[#This Row],[HP]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[HP]))</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="P2" t="str">
         <f ca="1">_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Ability])</f>
-        <v>Scorch</v>
+        <v>Pollinate</v>
       </c>
       <c r="Q2" s="7">
         <f ca="1">(Table8[[#This Row],[PP2]]+(Table8[[#This Row],[HP2]]/2)+IF(Table8[[#This Row],[Ability 1]]=0,0,1)+IF(Table8[[#This Row],[Ability 2]]=0,0,1))/(Table8[[#This Row],[Cost]]+1)</f>
-        <v>2.6</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -8836,15 +9073,15 @@
       </c>
       <c r="B3" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table8[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table8[[#This Row],[Type]])+1)))</f>
-        <v>Radi</v>
+        <v>Ura</v>
       </c>
       <c r="C3" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table8[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table8[[#This Row],[Type]])+1)))</f>
-        <v>theum</v>
+        <v>neon</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Raditheum</v>
+        <v>Uraneon</v>
       </c>
       <c r="E3">
         <f ca="1">SUM(_xlfn.XLOOKUP(Table8[[#This Row],[Generator]],Table2[Name],Table2[Cost]),_xlfn.XLOOKUP(Table8[[#This Row],[Frame]],Table1[Name],Table1[Cost]))</f>
@@ -8852,19 +9089,19 @@
       </c>
       <c r="F3">
         <f ca="1">_xlfn.XLOOKUP(B3,Table2[Name],Table2[PP])</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G3">
         <f ca="1">_xlfn.XLOOKUP(C3,Table1[Name],Table1[HP])</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H3" t="str">
         <f ca="1">_xlfn.XLOOKUP(B3,Table2[Name],Table2[Abiliity])</f>
         <v>Mutate</v>
       </c>
-      <c r="I3" t="str">
+      <c r="I3">
         <f ca="1">_xlfn.XLOOKUP(C3,Table1[Name],Table1[Ability])</f>
-        <v>Mutate</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <f ca="1">(Table8[[#This Row],[PP]]+(Table8[[#This Row],[HP]]/2)+IF(Table8[[#This Row],[Ability 1]]=0,0,1)+IF(Table8[[#This Row],[Ability 2]]=0,0,1))/(Table8[[#This Row],[Cost]]+1)</f>
@@ -8872,11 +9109,11 @@
       </c>
       <c r="K3" t="str" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>xi</v>
+        <v>pe</v>
       </c>
       <c r="L3" t="str">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
-        <v>Radixitheum</v>
+        <v>Urapeneon</v>
       </c>
       <c r="M3">
         <f ca="1">SUM(Table8[[#This Row],[Cost]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Cost]))</f>
@@ -8884,15 +9121,15 @@
       </c>
       <c r="N3">
         <f ca="1">SUM(Table8[[#This Row],[PP]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[PP]))</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O3">
         <f ca="1">SUM(Table8[[#This Row],[HP]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[HP]))</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P3" t="str">
         <f ca="1">_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Ability])</f>
-        <v>Burn</v>
+        <v>Pack</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">(Table8[[#This Row],[PP2]]+(Table8[[#This Row],[HP2]]/2)+IF(Table8[[#This Row],[Ability 1]]=0,0,1)+IF(Table8[[#This Row],[Ability 2]]=0,0,1))/(Table8[[#This Row],[Cost]]+1)</f>
@@ -8941,11 +9178,11 @@
       </c>
       <c r="K4" t="str" cm="1">
         <f t="array" aca="1" ref="K4" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>ro</v>
+        <v>tau</v>
       </c>
       <c r="L4" t="str" cm="1">
         <f t="array" aca="1" ref="L4" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>be</v>
+        <v>de</v>
       </c>
       <c r="M4">
         <f ca="1">SUM(Table8[[#This Row],[Cost]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Cost]))</f>
@@ -8961,7 +9198,7 @@
       </c>
       <c r="P4" t="str">
         <f ca="1">_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Ability])</f>
-        <v>Mutate</v>
+        <v>Flattery</v>
       </c>
       <c r="Q4" s="7">
         <f ca="1">(Table8[[#This Row],[PP2]]+(Table8[[#This Row],[HP2]]/2)+IF(Table8[[#This Row],[Ability 1]]=0,0,1)+IF(Table8[[#This Row],[Ability 2]]=0,0,1))/(Table8[[#This Row],[Cost]]+1)</f>
@@ -8974,15 +9211,15 @@
       </c>
       <c r="B5" t="str" cm="1">
         <f t="array" aca="1" ref="B5" ca="1">INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table8[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table8[[#This Row],[Type]])+1)))</f>
-        <v>Explo</v>
+        <v>Thurma</v>
       </c>
       <c r="C5" t="str" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table8[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table8[[#This Row],[Type]])+1)))</f>
-        <v>gul</v>
+        <v>tus</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Explogul</v>
+        <v>Thurmatus</v>
       </c>
       <c r="E5">
         <f ca="1">SUM(_xlfn.XLOOKUP(Table8[[#This Row],[Generator]],Table2[Name],Table2[Cost]),_xlfn.XLOOKUP(Table8[[#This Row],[Frame]],Table1[Name],Table1[Cost]))</f>
@@ -8990,11 +9227,11 @@
       </c>
       <c r="F5">
         <f ca="1">_xlfn.XLOOKUP(B5,Table2[Name],Table2[PP])</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G5">
         <f ca="1">_xlfn.XLOOKUP(C5,Table1[Name],Table1[HP])</f>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H5" t="str">
         <f ca="1">_xlfn.XLOOKUP(B5,Table2[Name],Table2[Abiliity])</f>
@@ -9002,19 +9239,19 @@
       </c>
       <c r="I5" t="str">
         <f ca="1">_xlfn.XLOOKUP(C5,Table1[Name],Table1[Ability])</f>
-        <v>Scorch</v>
+        <v>Burn</v>
       </c>
       <c r="J5">
         <f ca="1">(Table8[[#This Row],[PP]]+(Table8[[#This Row],[HP]]/2)+IF(Table8[[#This Row],[Ability 1]]=0,0,1)+IF(Table8[[#This Row],[Ability 2]]=0,0,1))/(Table8[[#This Row],[Cost]]+1)</f>
-        <v>2.6</v>
+        <v>2.4</v>
       </c>
       <c r="K5" t="str" cm="1">
         <f t="array" aca="1" ref="K5" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>pi</v>
+        <v>pu</v>
       </c>
       <c r="L5" t="str">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
-        <v>Explopigul</v>
+        <v>Thurmaputus</v>
       </c>
       <c r="M5">
         <f ca="1">SUM(Table8[[#This Row],[Cost]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Cost]))</f>
@@ -9022,19 +9259,19 @@
       </c>
       <c r="N5">
         <f ca="1">SUM(Table8[[#This Row],[PP]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[PP]))</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O5">
         <f ca="1">SUM(Table8[[#This Row],[HP]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[HP]))</f>
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="P5" t="str">
         <f ca="1">_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Ability])</f>
-        <v>Burn</v>
+        <v>Barrier</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">(Table8[[#This Row],[PP2]]+(Table8[[#This Row],[HP2]]/2)+IF(Table8[[#This Row],[Ability 1]]=0,0,1)+IF(Table8[[#This Row],[Ability 2]]=0,0,1))/(Table8[[#This Row],[Cost]]+1)</f>
-        <v>3</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -9043,15 +9280,15 @@
       </c>
       <c r="B6" t="str" cm="1">
         <f t="array" aca="1" ref="B6" ca="1">INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table8[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table8[[#This Row],[Type]])+1)))</f>
-        <v>Carni</v>
+        <v>Fauna</v>
       </c>
       <c r="C6" t="str" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table8[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table8[[#This Row],[Type]])+1)))</f>
-        <v>ctos</v>
+        <v>ling</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Carnictos</v>
+        <v>Faunaling</v>
       </c>
       <c r="E6">
         <f ca="1">SUM(_xlfn.XLOOKUP(Table8[[#This Row],[Generator]],Table2[Name],Table2[Cost]),_xlfn.XLOOKUP(Table8[[#This Row],[Frame]],Table1[Name],Table1[Cost]))</f>
@@ -9059,31 +9296,31 @@
       </c>
       <c r="F6">
         <f ca="1">_xlfn.XLOOKUP(B6,Table2[Name],Table2[PP])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G6">
         <f ca="1">_xlfn.XLOOKUP(C6,Table1[Name],Table1[HP])</f>
-        <v>6</v>
-      </c>
-      <c r="H6" t="str">
+        <v>4</v>
+      </c>
+      <c r="H6">
         <f ca="1">_xlfn.XLOOKUP(B6,Table2[Name],Table2[Abiliity])</f>
-        <v>Pack</v>
-      </c>
-      <c r="I6" t="str">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <f ca="1">_xlfn.XLOOKUP(C6,Table1[Name],Table1[Ability])</f>
-        <v>Pack</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <f ca="1">(Table8[[#This Row],[PP]]+(Table8[[#This Row],[HP]]/2)+IF(Table8[[#This Row],[Ability 1]]=0,0,1)+IF(Table8[[#This Row],[Ability 2]]=0,0,1))/(Table8[[#This Row],[Cost]]+1)</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="K6" t="str" cm="1">
         <f t="array" aca="1" ref="K6" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>mu</v>
+        <v>zi</v>
       </c>
       <c r="L6" t="str">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
-        <v>Carnimuctos</v>
+        <v>Faunaziling</v>
       </c>
       <c r="M6">
         <f ca="1">SUM(Table8[[#This Row],[Cost]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Cost]))</f>
@@ -9091,19 +9328,19 @@
       </c>
       <c r="N6">
         <f ca="1">SUM(Table8[[#This Row],[PP]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[PP]))</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O6">
         <f ca="1">SUM(Table8[[#This Row],[HP]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[HP]))</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="P6" t="str">
         <f ca="1">_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Ability])</f>
-        <v>Mutate</v>
+        <v>None</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">(Table8[[#This Row],[PP2]]+(Table8[[#This Row],[HP2]]/2)+IF(Table8[[#This Row],[Ability 1]]=0,0,1)+IF(Table8[[#This Row],[Ability 2]]=0,0,1))/(Table8[[#This Row],[Cost]]+1)</f>
-        <v>4.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -9112,27 +9349,27 @@
       </c>
       <c r="B7" t="str" cm="1">
         <f t="array" aca="1" ref="B7" ca="1">INDEX(Table2[Name],LARGE(IF(Table2[Type]=Table8[[#This Row],[Type]],ROW(Table2[Type])-1),INT(RAND()*COUNTIF(Table2[Type],Table8[[#This Row],[Type]])+1)))</f>
-        <v>Mega</v>
+        <v>Ultra</v>
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Type]=Table8[[#This Row],[Type]],ROW(Table1[Type])-1),INT(RAND()*COUNTIF(Table1[Type],Table8[[#This Row],[Type]])+1)))</f>
-        <v>cell</v>
+        <v>shell</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Megacell</v>
+        <v>Ultrashell</v>
       </c>
       <c r="E7">
         <f ca="1">SUM(_xlfn.XLOOKUP(Table8[[#This Row],[Generator]],Table2[Name],Table2[Cost]),_xlfn.XLOOKUP(Table8[[#This Row],[Frame]],Table1[Name],Table1[Cost]))</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F7">
         <f ca="1">_xlfn.XLOOKUP(B7,Table2[Name],Table2[PP])</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G7">
         <f ca="1">_xlfn.XLOOKUP(C7,Table1[Name],Table1[HP])</f>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H7">
         <f ca="1">_xlfn.XLOOKUP(B7,Table2[Name],Table2[Abiliity])</f>
@@ -9144,35 +9381,35 @@
       </c>
       <c r="J7">
         <f ca="1">(Table8[[#This Row],[PP]]+(Table8[[#This Row],[HP]]/2)+IF(Table8[[#This Row],[Ability 1]]=0,0,1)+IF(Table8[[#This Row],[Ability 2]]=0,0,1))/(Table8[[#This Row],[Cost]]+1)</f>
-        <v>3.6666666666666665</v>
+        <v>3</v>
       </c>
       <c r="K7" t="str" cm="1">
         <f t="array" aca="1" ref="K7" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>xi</v>
+        <v>pe</v>
       </c>
       <c r="L7" t="str">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
-        <v>Megaxicell</v>
+        <v>Ultrapeshell</v>
       </c>
       <c r="M7">
         <f ca="1">SUM(Table8[[#This Row],[Cost]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Cost]))</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N7">
         <f ca="1">SUM(Table8[[#This Row],[PP]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[PP]))</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="O7">
         <f ca="1">SUM(Table8[[#This Row],[HP]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[HP]))</f>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="P7" t="str">
         <f ca="1">_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Ability])</f>
-        <v>Burn</v>
+        <v>Pack</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">(Table8[[#This Row],[PP2]]+(Table8[[#This Row],[HP2]]/2)+IF(Table8[[#This Row],[Ability 1]]=0,0,1)+IF(Table8[[#This Row],[Ability 2]]=0,0,1))/(Table8[[#This Row],[Cost]]+1)</f>
-        <v>4.333333333333333</v>
+        <v>3.3333333333333335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor actions, add in more abilities, write pp gen function
</commit_message>
<xml_diff>
--- a/Excel/BotBuilder 2.0.xlsx
+++ b/Excel/BotBuilder 2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Fragment\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FA4DBF-6786-4A07-8D72-8E5C969C6A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232BA6C8-8672-4018-BE7B-56D236CFFAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8281E10D-33EF-4D46-A534-1BAF9E624D7F}"/>
   </bookViews>
@@ -571,9 +571,6 @@
     <t>Radiate</t>
   </si>
   <si>
-    <t>1 dmg to random enemy each time this bot attacks</t>
-  </si>
-  <si>
     <t>Tinder</t>
   </si>
   <si>
@@ -616,9 +613,6 @@
     <t>Rejig</t>
   </si>
   <si>
-    <t>Stun opponents on attack</t>
-  </si>
-  <si>
     <t>Whirlwind</t>
   </si>
   <si>
@@ -872,6 +866,12 @@
   </si>
   <si>
     <t>Deck</t>
+  </si>
+  <si>
+    <t>1 dmg to random enemy bot each time this bot attacks</t>
+  </si>
+  <si>
+    <t>Stun opponents when attacked</t>
   </si>
 </sst>
 </file>
@@ -1445,6 +1445,15 @@
     <xf numFmtId="0" fontId="8" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1455,15 +1464,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3333,7 +3333,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3349,7 +3349,7 @@
         <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C1" t="s">
         <v>30</v>
@@ -3379,7 +3379,7 @@
         <v>162</v>
       </c>
       <c r="F2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3397,7 +3397,7 @@
         <v>162</v>
       </c>
       <c r="F3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I3" s="47"/>
     </row>
@@ -3416,7 +3416,7 @@
         <v>162</v>
       </c>
       <c r="F4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I4" s="47"/>
     </row>
@@ -3435,7 +3435,7 @@
         <v>162</v>
       </c>
       <c r="F5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I5" s="47"/>
     </row>
@@ -3454,13 +3454,13 @@
         <v>162</v>
       </c>
       <c r="F6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I6" s="48"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -3473,21 +3473,21 @@
         <v>162</v>
       </c>
       <c r="F7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I7" s="46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J7" s="46" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D8" t="str">
         <f>"-1 PP to play mechanic cards"</f>
@@ -3497,7 +3497,7 @@
         <v>159</v>
       </c>
       <c r="F8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I8" s="46" t="s">
         <v>66</v>
@@ -3584,7 +3584,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
@@ -3634,7 +3634,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
@@ -3650,7 +3650,7 @@
         <v>2</v>
       </c>
       <c r="I14" s="46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J14" s="46">
         <f>COUNTIF(Table4[Resource],I14)</f>
@@ -3659,10 +3659,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D15" t="str">
         <f>"+2 HP each time you play a mechanic card"</f>
@@ -3690,7 +3690,7 @@
         <v>162</v>
       </c>
       <c r="F16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3708,12 +3708,12 @@
         <v>162</v>
       </c>
       <c r="F17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -3726,12 +3726,12 @@
         <v>162</v>
       </c>
       <c r="F18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
@@ -3744,12 +3744,12 @@
         <v>162</v>
       </c>
       <c r="F19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -3762,12 +3762,12 @@
         <v>162</v>
       </c>
       <c r="F20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
@@ -3780,15 +3780,15 @@
         <v>162</v>
       </c>
       <c r="F21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D22" t="str">
         <f>"+2 PP whenever an opponent plays a mechanic card"</f>
@@ -3798,7 +3798,7 @@
         <v>159</v>
       </c>
       <c r="F22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3816,7 +3816,7 @@
         <v>162</v>
       </c>
       <c r="F23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3831,10 +3831,10 @@
         <v>+1 PP per turn for each upgrade on this bot</v>
       </c>
       <c r="E24" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3845,13 +3845,13 @@
         <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E25" t="s">
         <v>162</v>
       </c>
       <c r="F25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -3866,10 +3866,10 @@
         <v>+1 PP from each non-adjacent Weather Event resource</v>
       </c>
       <c r="E26" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -3884,15 +3884,15 @@
         <v>+1 PP each turn for each active friendly bot</v>
       </c>
       <c r="E27" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B28" t="s">
         <v>17</v>
@@ -3905,15 +3905,15 @@
         <v>159</v>
       </c>
       <c r="F28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D29" t="str">
         <f>"+2 PP each time an enemy bot is destroyed"</f>
@@ -3923,7 +3923,7 @@
         <v>159</v>
       </c>
       <c r="F29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -3940,7 +3940,7 @@
         <v>162</v>
       </c>
       <c r="F30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -3955,10 +3955,10 @@
         <v>+1 dmg dealt for each upgrade on this bot</v>
       </c>
       <c r="E31" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -3969,30 +3969,30 @@
         <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>166</v>
+        <v>265</v>
       </c>
       <c r="E32" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F32" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B33" t="s">
         <v>37</v>
       </c>
       <c r="D33" t="s">
-        <v>181</v>
+        <v>266</v>
       </c>
       <c r="E33" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -4010,7 +4010,7 @@
         <v>159</v>
       </c>
       <c r="F34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -4021,22 +4021,22 @@
         <v>17</v>
       </c>
       <c r="D35" t="str">
-        <f>"-1 dmg to first attack each turn against this bot"</f>
-        <v>-1 dmg to first attack each turn against this bot</v>
+        <f>"-1 dmg to each attack against this bot"</f>
+        <v>-1 dmg to each attack against this bot</v>
       </c>
       <c r="E35" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F35" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D36" t="str">
         <f>"+1 effect for mechanic cards"</f>
@@ -4046,7 +4046,7 @@
         <v>159</v>
       </c>
       <c r="F36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -4079,10 +4079,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4141,7 +4141,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8" t="str">
         <f>"+1 from all resources"</f>
@@ -4184,7 +4184,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B2" s="50" t="s">
         <v>66</v>
@@ -4193,124 +4193,124 @@
         <v>2</v>
       </c>
       <c r="D2" s="50" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C3" s="51">
         <v>1</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C4" s="50">
         <v>3</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="51" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C5" s="51">
         <v>2</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="50" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C6" s="50">
         <v>4</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C7" s="51">
         <v>1</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C8" s="50">
         <v>2</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="51" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C9" s="51">
         <v>3</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C10" s="50">
         <v>4</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B11" s="51" t="s">
         <v>4</v>
@@ -4319,12 +4319,12 @@
         <v>1</v>
       </c>
       <c r="D11" s="51" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="50" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B12" s="50" t="s">
         <v>7</v>
@@ -4333,12 +4333,12 @@
         <v>1</v>
       </c>
       <c r="D12" s="50" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B13" s="51" t="s">
         <v>37</v>
@@ -4347,12 +4347,12 @@
         <v>1</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B14" s="51" t="s">
         <v>11</v>
@@ -4361,7 +4361,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -4375,21 +4375,21 @@
         <v>2</v>
       </c>
       <c r="D15" s="50" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" s="50" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -4420,7 +4420,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C1" s="52" t="s">
         <v>30</v>
@@ -4429,10 +4429,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="52" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -4490,7 +4490,7 @@
         <v>66</v>
       </c>
       <c r="F4" s="53" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -4530,7 +4530,7 @@
         <v>66</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -4653,7 +4653,7 @@
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B13" s="61" t="s">
         <v>4</v>
@@ -4668,12 +4668,12 @@
         <v>4</v>
       </c>
       <c r="F13" s="60" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B14" s="63" t="s">
         <v>7</v>
@@ -4711,7 +4711,7 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="64" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B16" s="65" t="s">
         <v>7</v>
@@ -4726,7 +4726,7 @@
         <v>7</v>
       </c>
       <c r="F16" s="64" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -4824,7 +4824,7 @@
         <v>37</v>
       </c>
       <c r="F21" s="68" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -4884,7 +4884,7 @@
         <v>37</v>
       </c>
       <c r="F24" s="66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -4982,7 +4982,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="70" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5027,7 +5027,7 @@
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="74" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B32" s="75" t="s">
         <v>17</v>
@@ -5045,7 +5045,7 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="76" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B33" s="77" t="s">
         <v>17</v>
@@ -5065,7 +5065,7 @@
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="74" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B34" s="75" t="s">
         <v>17</v>
@@ -5080,12 +5080,12 @@
         <v>17</v>
       </c>
       <c r="F34" s="74" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="76" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B35" s="77" t="s">
         <v>17</v>
@@ -5100,7 +5100,7 @@
         <v>17</v>
       </c>
       <c r="F35" s="76" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5120,7 +5120,7 @@
         <v>17</v>
       </c>
       <c r="F36" s="74" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5140,15 +5140,15 @@
         <v>17</v>
       </c>
       <c r="F37" s="74" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C38" s="17">
         <v>1</v>
@@ -5157,16 +5157,16 @@
         <v>2</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F38" s="17"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C39" s="17">
         <v>2</v>
@@ -5175,18 +5175,18 @@
         <v>4</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C40" s="17">
         <v>2</v>
@@ -5195,18 +5195,18 @@
         <v>4</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C41" s="17">
         <v>2</v>
@@ -5215,18 +5215,18 @@
         <v>4</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F41" s="78" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C42" s="17">
         <v>2</v>
@@ -5235,18 +5235,18 @@
         <v>4</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F42" s="78" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C43" s="17">
         <v>2</v>
@@ -5255,10 +5255,10 @@
         <v>4</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F43" s="78" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -5318,7 +5318,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C1" s="52" t="s">
         <v>30</v>
@@ -5327,10 +5327,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="52" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -5347,10 +5347,10 @@
         <v>8</v>
       </c>
       <c r="E2" s="53" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F2" s="53" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5367,10 +5367,10 @@
         <v>8</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F3" s="56" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -5387,10 +5387,10 @@
         <v>8</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F4" s="53" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -5407,10 +5407,10 @@
         <v>8</v>
       </c>
       <c r="E5" s="56" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F5" s="56" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -5427,10 +5427,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F6" s="53" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -5447,10 +5447,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F7" s="56" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -5467,10 +5467,10 @@
         <v>8</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F8" s="53" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -5487,10 +5487,10 @@
         <v>8</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F9" s="56" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -5507,10 +5507,10 @@
         <v>8</v>
       </c>
       <c r="E10" s="58" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F10" s="58" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -5527,10 +5527,10 @@
         <v>8</v>
       </c>
       <c r="E11" s="60" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F11" s="60" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -5547,10 +5547,10 @@
         <v>8</v>
       </c>
       <c r="E12" s="58" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F12" s="58" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -5567,10 +5567,10 @@
         <v>8</v>
       </c>
       <c r="E13" s="60" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F13" s="60" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -5587,10 +5587,10 @@
         <v>8</v>
       </c>
       <c r="E14" s="58" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F14" s="58" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -5607,10 +5607,10 @@
         <v>8</v>
       </c>
       <c r="E15" s="60" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F15" s="60" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -5627,10 +5627,10 @@
         <v>8</v>
       </c>
       <c r="E16" s="58" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F16" s="58" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -5647,10 +5647,10 @@
         <v>8</v>
       </c>
       <c r="E17" s="60" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F17" s="60" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -5667,10 +5667,10 @@
         <v>8</v>
       </c>
       <c r="E18" s="62" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F18" s="62" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -5687,10 +5687,10 @@
         <v>8</v>
       </c>
       <c r="E19" s="64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F19" s="64" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -5707,10 +5707,10 @@
         <v>8</v>
       </c>
       <c r="E20" s="62" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F20" s="62" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -5727,10 +5727,10 @@
         <v>8</v>
       </c>
       <c r="E21" s="64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F21" s="64" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -5747,10 +5747,10 @@
         <v>8</v>
       </c>
       <c r="E22" s="62" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F22" s="62" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -5767,10 +5767,10 @@
         <v>8</v>
       </c>
       <c r="E23" s="64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F23" s="64" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -5787,10 +5787,10 @@
         <v>8</v>
       </c>
       <c r="E24" s="62" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F24" s="62" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -5807,10 +5807,10 @@
         <v>8</v>
       </c>
       <c r="E25" s="64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F25" s="64" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -5827,10 +5827,10 @@
         <v>8</v>
       </c>
       <c r="E26" s="66" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F26" s="66" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -5847,10 +5847,10 @@
         <v>8</v>
       </c>
       <c r="E27" s="68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F27" s="68" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -5867,10 +5867,10 @@
         <v>8</v>
       </c>
       <c r="E28" s="66" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F28" s="66" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -5887,10 +5887,10 @@
         <v>8</v>
       </c>
       <c r="E29" s="68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F29" s="68" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -5907,10 +5907,10 @@
         <v>8</v>
       </c>
       <c r="E30" s="68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F30" s="66" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -5927,10 +5927,10 @@
         <v>8</v>
       </c>
       <c r="E31" s="68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F31" s="68" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -5947,10 +5947,10 @@
         <v>8</v>
       </c>
       <c r="E32" s="68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F32" s="66" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -5967,10 +5967,10 @@
         <v>8</v>
       </c>
       <c r="E33" s="68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F33" s="68" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -5987,10 +5987,10 @@
         <v>8</v>
       </c>
       <c r="E34" s="70" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F34" s="70" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -6007,10 +6007,10 @@
         <v>8</v>
       </c>
       <c r="E35" s="72" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F35" s="72" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -6027,10 +6027,10 @@
         <v>8</v>
       </c>
       <c r="E36" s="70" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F36" s="70" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -6047,15 +6047,15 @@
         <v>8</v>
       </c>
       <c r="E37" s="72" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F37" s="72" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="70" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B38" s="71" t="s">
         <v>11</v>
@@ -6067,10 +6067,10 @@
         <v>8</v>
       </c>
       <c r="E38" s="70" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F38" s="70" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -6087,10 +6087,10 @@
         <v>8</v>
       </c>
       <c r="E39" s="72" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F39" s="72" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -6107,10 +6107,10 @@
         <v>8</v>
       </c>
       <c r="E40" s="70" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F40" s="70" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -6127,10 +6127,10 @@
         <v>8</v>
       </c>
       <c r="E41" s="72" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F41" s="72" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -6150,7 +6150,7 @@
         <v>77</v>
       </c>
       <c r="F42" s="74" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -6170,7 +6170,7 @@
         <v>77</v>
       </c>
       <c r="F43" s="76" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -6190,7 +6190,7 @@
         <v>77</v>
       </c>
       <c r="F44" s="74" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -6210,7 +6210,7 @@
         <v>77</v>
       </c>
       <c r="F45" s="76" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -6230,7 +6230,7 @@
         <v>77</v>
       </c>
       <c r="F46" s="74" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -6250,7 +6250,7 @@
         <v>77</v>
       </c>
       <c r="F47" s="76" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -6270,7 +6270,7 @@
         <v>77</v>
       </c>
       <c r="F48" s="74" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -6290,15 +6290,15 @@
         <v>77</v>
       </c>
       <c r="F49" s="76" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="16" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C50" s="16">
         <v>3</v>
@@ -6307,18 +6307,18 @@
         <v>8</v>
       </c>
       <c r="E50" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F50" s="16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C51" s="16">
         <v>3</v>
@@ -6327,18 +6327,18 @@
         <v>8</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="16" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C52" s="16">
         <v>3</v>
@@ -6347,18 +6347,18 @@
         <v>8</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F52" s="16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="16" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C53" s="16">
         <v>3</v>
@@ -6367,18 +6367,18 @@
         <v>8</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C54" s="16">
         <v>3</v>
@@ -6387,18 +6387,18 @@
         <v>8</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="16" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C55" s="16">
         <v>3</v>
@@ -6407,18 +6407,18 @@
         <v>8</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="16" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C56" s="16">
         <v>3</v>
@@ -6427,18 +6427,18 @@
         <v>8</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F56" s="16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C57" s="16">
         <v>3</v>
@@ -6447,10 +6447,10 @@
         <v>8</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F57" s="16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -6486,7 +6486,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="79" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -6500,7 +6500,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="81" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -6514,7 +6514,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="82" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -6528,7 +6528,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="81" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -6542,7 +6542,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="82" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -6556,7 +6556,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="81" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -6570,12 +6570,12 @@
         <v>4</v>
       </c>
       <c r="D7" s="82" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="81" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B8" s="81">
         <v>2</v>
@@ -6584,12 +6584,12 @@
         <v>4</v>
       </c>
       <c r="D8" s="81" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="82" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B9" s="82">
         <v>2</v>
@@ -6598,12 +6598,12 @@
         <v>4</v>
       </c>
       <c r="D9" s="82" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="81" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B10" s="81">
         <v>2</v>
@@ -6612,12 +6612,12 @@
         <v>4</v>
       </c>
       <c r="D10" s="81" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="82" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B11" s="82">
         <v>2</v>
@@ -6626,12 +6626,12 @@
         <v>4</v>
       </c>
       <c r="D11" s="82" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="81" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B12" s="81">
         <v>2</v>
@@ -6640,12 +6640,12 @@
         <v>4</v>
       </c>
       <c r="D12" s="81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="82" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B13" s="82">
         <v>2</v>
@@ -6654,12 +6654,12 @@
         <v>4</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="81" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B14" s="81">
         <v>2</v>
@@ -6673,7 +6673,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="82" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B15" s="82">
         <v>2</v>
@@ -6682,12 +6682,12 @@
         <v>4</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="81" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B16" s="81">
         <v>2</v>
@@ -6735,34 +6735,34 @@
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="85"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="88"/>
       <c r="H2" s="14"/>
-      <c r="I2" s="83" t="s">
+      <c r="I2" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="85"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="88"/>
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="83" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="87" t="s">
+      <c r="C3" s="84"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="83" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="88"/>
-      <c r="G3" s="89"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="85"/>
       <c r="H3" s="15"/>
       <c r="I3" s="39" t="s">
         <v>111</v>
@@ -7038,40 +7038,40 @@
     </row>
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="86" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="84"/>
-      <c r="J12" s="85"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="88"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
       <c r="M12" s="14"/>
     </row>
     <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="88"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="87" t="s">
+      <c r="C13" s="84"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="88"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="87" t="s">
+      <c r="F13" s="84"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="83" t="s">
         <v>114</v>
       </c>
-      <c r="I13" s="88"/>
-      <c r="J13" s="89"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="85"/>
       <c r="K13" s="38"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="86"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="89"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -7454,42 +7454,42 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="83" t="s">
+      <c r="B22" s="86" t="s">
         <v>129</v>
       </c>
-      <c r="C22" s="84"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="84"/>
-      <c r="F22" s="84"/>
-      <c r="G22" s="84"/>
-      <c r="H22" s="84"/>
-      <c r="I22" s="84"/>
-      <c r="J22" s="84"/>
-      <c r="K22" s="84"/>
-      <c r="L22" s="84"/>
-      <c r="M22" s="85"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="87"/>
+      <c r="K22" s="87"/>
+      <c r="L22" s="87"/>
+      <c r="M22" s="88"/>
     </row>
     <row r="23" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="87" t="s">
+      <c r="B23" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="88"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="87" t="s">
+      <c r="C23" s="84"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="88"/>
-      <c r="G23" s="89"/>
-      <c r="H23" s="87" t="s">
+      <c r="F23" s="84"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="83" t="s">
         <v>114</v>
       </c>
-      <c r="I23" s="88"/>
-      <c r="J23" s="89"/>
-      <c r="K23" s="87" t="s">
+      <c r="I23" s="84"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="L23" s="88"/>
-      <c r="M23" s="89"/>
+      <c r="L23" s="84"/>
+      <c r="M23" s="85"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
@@ -7828,12 +7828,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B22:M22"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="M13:N13"/>
@@ -7842,6 +7836,12 @@
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B22:M22"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:G10">
     <cfRule type="dataBar" priority="44">
@@ -8291,7 +8291,7 @@
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>nacht</v>
+        <v>fel</v>
       </c>
       <c r="D2" t="e">
         <f t="shared" ref="D2:D7" ca="1" si="0">_xlfn.CONCAT(B2,C2)</f>
@@ -8323,7 +8323,7 @@
       </c>
       <c r="K2" t="str" cm="1">
         <f t="array" aca="1" ref="K2" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Turbo</v>
+        <v>Hasta</v>
       </c>
       <c r="L2" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
@@ -8360,7 +8360,7 @@
       </c>
       <c r="C3" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>lium</v>
+        <v>theum</v>
       </c>
       <c r="D3" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8392,7 +8392,7 @@
       </c>
       <c r="K3" t="str" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Muta</v>
+        <v>Blasta</v>
       </c>
       <c r="L3" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
@@ -8429,7 +8429,7 @@
       </c>
       <c r="C4" t="str" cm="1">
         <f t="array" aca="1" ref="C4" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>morph</v>
+        <v>mant</v>
       </c>
       <c r="D4" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8461,11 +8461,11 @@
       </c>
       <c r="K4" t="str" cm="1">
         <f t="array" aca="1" ref="K4" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Multi</v>
+        <v>Dima</v>
       </c>
       <c r="L4" t="str" cm="1">
         <f t="array" aca="1" ref="L4" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Meta</v>
+        <v>Turbo</v>
       </c>
       <c r="M4" t="e">
         <f ca="1">SUM(Table8[[#This Row],[Cost]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Cost]))</f>
@@ -8498,7 +8498,7 @@
       </c>
       <c r="C5" t="str" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>lus</v>
+        <v>don</v>
       </c>
       <c r="D5" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8530,7 +8530,7 @@
       </c>
       <c r="K5" t="str" cm="1">
         <f t="array" aca="1" ref="K5" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Shello</v>
+        <v>Multi</v>
       </c>
       <c r="L5" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
@@ -8567,7 +8567,7 @@
       </c>
       <c r="C6" t="str" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>pod</v>
+        <v>ctos</v>
       </c>
       <c r="D6" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8599,7 +8599,7 @@
       </c>
       <c r="K6" t="str" cm="1">
         <f t="array" aca="1" ref="K6" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Supra</v>
+        <v>Giga</v>
       </c>
       <c r="L6" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
@@ -8668,7 +8668,7 @@
       </c>
       <c r="K7" t="str" cm="1">
         <f t="array" aca="1" ref="K7" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Supra</v>
+        <v>Tera</v>
       </c>
       <c r="L7" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>

</xml_diff>

<commit_message>
Debug game manager code
</commit_message>
<xml_diff>
--- a/Excel/BotBuilder 2.0.xlsx
+++ b/Excel/BotBuilder 2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Fragment\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232BA6C8-8672-4018-BE7B-56D236CFFAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BB3FBC-6056-48FE-B9B8-C5C8F29C1FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8281E10D-33EF-4D46-A534-1BAF9E624D7F}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="269">
   <si>
     <t>Name</t>
   </si>
@@ -872,6 +872,12 @@
   </si>
   <si>
     <t>Stun opponents when attacked</t>
+  </si>
+  <si>
+    <t>(Stackable?)</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -1445,15 +1451,6 @@
     <xf numFmtId="0" fontId="8" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1464,6 +1461,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2752,18 +2758,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E37455DC-4ECB-45E2-A2F6-20EE7804BD41}" name="Table4" displayName="Table4" ref="A1:F36" totalsRowShown="0">
-  <autoFilter ref="A1:F36" xr:uid="{E37455DC-4ECB-45E2-A2F6-20EE7804BD41}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E37455DC-4ECB-45E2-A2F6-20EE7804BD41}" name="Table4" displayName="Table4" ref="A1:G36" totalsRowShown="0">
+  <autoFilter ref="A1:G36" xr:uid="{E37455DC-4ECB-45E2-A2F6-20EE7804BD41}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F36">
     <sortCondition ref="F1:F36"/>
   </sortState>
-  <tableColumns count="6">
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{2C2DC5BE-3D53-4039-B785-CD3E08BDFCBF}" name="Ability"/>
     <tableColumn id="3" xr3:uid="{DA21F8AF-9033-4E1F-891A-27F44C9FC291}" name="Resource"/>
     <tableColumn id="4" xr3:uid="{09B4F176-D59A-4F03-81BE-AB862B687D40}" name="Cost"/>
     <tableColumn id="2" xr3:uid="{1A297FB4-49E2-4175-9072-88EEAE7031DC}" name="Effect"/>
     <tableColumn id="5" xr3:uid="{DAE354FE-0FBE-44C2-BEB2-C21E3CC3646D}" name="Coded?"/>
     <tableColumn id="6" xr3:uid="{3EAB07D9-A5D5-46B0-A4CD-2304B0E828C1}" name="Type"/>
+    <tableColumn id="7" xr3:uid="{AEB82322-EFD5-4976-8DEF-3BF43CEC056B}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3332,8 +3339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798D3000-7536-4EA3-B16D-80887633F251}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3363,6 +3370,9 @@
       <c r="F1" t="s">
         <v>1</v>
       </c>
+      <c r="G1" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3902,7 +3912,7 @@
         <v>+2 PP each time a friendly bot is destroyed</v>
       </c>
       <c r="E28" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F28" t="s">
         <v>175</v>
@@ -3920,7 +3930,7 @@
         <v>+2 PP each time an enemy bot is destroyed</v>
       </c>
       <c r="E29" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F29" t="s">
         <v>175</v>
@@ -3978,7 +3988,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>180</v>
       </c>
@@ -3994,8 +4004,11 @@
       <c r="F33" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>149</v>
       </c>
@@ -4007,13 +4020,13 @@
         <v>+1 dmg to attacks for each bot you destroy</v>
       </c>
       <c r="E34" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F34" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -4031,7 +4044,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>179</v>
       </c>
@@ -6735,34 +6748,34 @@
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="88"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="85"/>
       <c r="H2" s="14"/>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="83" t="s">
         <v>144</v>
       </c>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="88"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="85"/>
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="83" t="s">
+      <c r="C3" s="88"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="87" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="84"/>
-      <c r="G3" s="85"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="89"/>
       <c r="H3" s="15"/>
       <c r="I3" s="39" t="s">
         <v>111</v>
@@ -7038,40 +7051,40 @@
     </row>
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="86" t="s">
+      <c r="B12" s="83" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="88"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="85"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
       <c r="M12" s="14"/>
     </row>
     <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="84"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="83" t="s">
+      <c r="C13" s="88"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="84"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="83" t="s">
+      <c r="F13" s="88"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="I13" s="84"/>
-      <c r="J13" s="85"/>
+      <c r="I13" s="88"/>
+      <c r="J13" s="89"/>
       <c r="K13" s="38"/>
-      <c r="M13" s="89"/>
-      <c r="N13" s="89"/>
+      <c r="M13" s="86"/>
+      <c r="N13" s="86"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -7454,42 +7467,42 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="86" t="s">
+      <c r="B22" s="83" t="s">
         <v>129</v>
       </c>
-      <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="87"/>
-      <c r="I22" s="87"/>
-      <c r="J22" s="87"/>
-      <c r="K22" s="87"/>
-      <c r="L22" s="87"/>
-      <c r="M22" s="88"/>
+      <c r="C22" s="84"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="84"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="84"/>
+      <c r="K22" s="84"/>
+      <c r="L22" s="84"/>
+      <c r="M22" s="85"/>
     </row>
     <row r="23" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="83" t="s">
+      <c r="B23" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="84"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="83" t="s">
+      <c r="C23" s="88"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="84"/>
-      <c r="G23" s="85"/>
-      <c r="H23" s="83" t="s">
+      <c r="F23" s="88"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="I23" s="84"/>
-      <c r="J23" s="85"/>
-      <c r="K23" s="83" t="s">
+      <c r="I23" s="88"/>
+      <c r="J23" s="89"/>
+      <c r="K23" s="87" t="s">
         <v>130</v>
       </c>
-      <c r="L23" s="84"/>
-      <c r="M23" s="85"/>
+      <c r="L23" s="88"/>
+      <c r="M23" s="89"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
@@ -7828,6 +7841,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B22:M22"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="M13:N13"/>
@@ -7836,12 +7855,6 @@
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:G3"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B22:M22"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:G10">
     <cfRule type="dataBar" priority="44">
@@ -8291,7 +8304,7 @@
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>fel</v>
+        <v>nacht</v>
       </c>
       <c r="D2" t="e">
         <f t="shared" ref="D2:D7" ca="1" si="0">_xlfn.CONCAT(B2,C2)</f>
@@ -8323,7 +8336,7 @@
       </c>
       <c r="K2" t="str" cm="1">
         <f t="array" aca="1" ref="K2" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Hasta</v>
+        <v>Dima</v>
       </c>
       <c r="L2" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
@@ -8360,7 +8373,7 @@
       </c>
       <c r="C3" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>theum</v>
+        <v>line</v>
       </c>
       <c r="D3" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8392,7 +8405,7 @@
       </c>
       <c r="K3" t="str" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Blasta</v>
+        <v>Supra</v>
       </c>
       <c r="L3" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
@@ -8429,7 +8442,7 @@
       </c>
       <c r="C4" t="str" cm="1">
         <f t="array" aca="1" ref="C4" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>mant</v>
+        <v>talus</v>
       </c>
       <c r="D4" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8461,11 +8474,11 @@
       </c>
       <c r="K4" t="str" cm="1">
         <f t="array" aca="1" ref="K4" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Dima</v>
+        <v>Meta</v>
       </c>
       <c r="L4" t="str" cm="1">
         <f t="array" aca="1" ref="L4" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Turbo</v>
+        <v>Shello</v>
       </c>
       <c r="M4" t="e">
         <f ca="1">SUM(Table8[[#This Row],[Cost]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Cost]))</f>
@@ -8498,7 +8511,7 @@
       </c>
       <c r="C5" t="str" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>don</v>
+        <v>ton</v>
       </c>
       <c r="D5" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8668,7 +8681,7 @@
       </c>
       <c r="K7" t="str" cm="1">
         <f t="array" aca="1" ref="K7" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Tera</v>
+        <v>Shello</v>
       </c>
       <c r="L7" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>

</xml_diff>

<commit_message>
"Import csv files and get game running"
</commit_message>
<xml_diff>
--- a/Excel/BotBuilder 2.0.xlsx
+++ b/Excel/BotBuilder 2.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Fragment\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SJWDa\Projects\Fragment\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BB3FBC-6056-48FE-B9B8-C5C8F29C1FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6CFC33-0D9B-4D47-AE47-24DFDFE90F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8281E10D-33EF-4D46-A534-1BAF9E624D7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{8281E10D-33EF-4D46-A534-1BAF9E624D7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Passive abilities" sheetId="4" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="268">
   <si>
     <t>Name</t>
   </si>
@@ -860,9 +860,6 @@
   </si>
   <si>
     <t>Action</t>
-  </si>
-  <si>
-    <t>Ability 12</t>
   </si>
   <si>
     <t>Deck</t>
@@ -1451,6 +1448,15 @@
     <xf numFmtId="0" fontId="8" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1461,15 +1467,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2819,7 +2816,7 @@
       <calculatedColumnFormula>_xlfn.XLOOKUP(C2,Table1[Name],Table1[HP])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{6A0D5295-BD65-4229-884E-D6CCB0F26C35}" name="Ability 1">
-      <calculatedColumnFormula>_xlfn.XLOOKUP(B2,Table2[Name],Table2[Ability 12])</calculatedColumnFormula>
+      <calculatedColumnFormula>_xlfn.XLOOKUP(B2,Table2[Name],Table2[Ability 1])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{D892DF1C-8138-4EB4-8C4C-A6F7B91F63C4}" name="Ability 2">
       <calculatedColumnFormula>_xlfn.XLOOKUP(C2,Table1[Name],Table1[Action 1])</calculatedColumnFormula>
@@ -2901,7 +2898,7 @@
     <tableColumn id="2" xr3:uid="{7AB76467-159E-460D-9139-B4222C9E583D}" name="Deck" dataDxfId="84"/>
     <tableColumn id="3" xr3:uid="{E017E39D-29F1-4E55-98B2-8FC221A535CB}" name="Cost"/>
     <tableColumn id="4" xr3:uid="{0C4B96A8-AEC8-4A0E-8BE8-D7CB34749D2F}" name="HP"/>
-    <tableColumn id="6" xr3:uid="{C3850DEF-7805-4A9E-9633-EEEB17887BC8}" name="Ability 12" dataDxfId="83"/>
+    <tableColumn id="6" xr3:uid="{C3850DEF-7805-4A9E-9633-EEEB17887BC8}" name="Ability 1" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3339,7 +3336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798D3000-7536-4EA3-B16D-80887633F251}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
@@ -3371,7 +3368,7 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3979,7 +3976,7 @@
         <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E32" t="s">
         <v>162</v>
@@ -3996,7 +3993,7 @@
         <v>37</v>
       </c>
       <c r="D33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E33" t="s">
         <v>162</v>
@@ -4005,7 +4002,7 @@
         <v>176</v>
       </c>
       <c r="G33" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -4417,8 +4414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A60404A-0BD4-4949-BF8C-296F3D670006}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4433,7 +4430,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C1" s="52" t="s">
         <v>30</v>
@@ -4442,7 +4439,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="52" t="s">
-        <v>263</v>
+        <v>93</v>
       </c>
       <c r="F1" s="52" t="s">
         <v>259</v>
@@ -5326,12 +5323,12 @@
     <col min="8" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C1" s="52" t="s">
         <v>30</v>
@@ -6748,34 +6745,34 @@
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="85"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="88"/>
       <c r="H2" s="14"/>
-      <c r="I2" s="83" t="s">
+      <c r="I2" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="85"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="88"/>
       <c r="M2" s="14"/>
     </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="87" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B3" s="83" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="87" t="s">
+      <c r="C3" s="84"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="83" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="88"/>
-      <c r="G3" s="89"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="85"/>
       <c r="H3" s="15"/>
       <c r="I3" s="39" t="s">
         <v>111</v>
@@ -6833,7 +6830,7 @@
       </c>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>66</v>
       </c>
@@ -6914,7 +6911,7 @@
       </c>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>7</v>
       </c>
@@ -7051,40 +7048,40 @@
     </row>
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="86" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="84"/>
-      <c r="J12" s="85"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="88"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="87" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B13" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="88"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="87" t="s">
+      <c r="C13" s="84"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="88"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="87" t="s">
+      <c r="F13" s="84"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="83" t="s">
         <v>114</v>
       </c>
-      <c r="I13" s="88"/>
-      <c r="J13" s="89"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="85"/>
       <c r="K13" s="38"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="86"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="89"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -7467,42 +7464,42 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="83" t="s">
+      <c r="B22" s="86" t="s">
         <v>129</v>
       </c>
-      <c r="C22" s="84"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="84"/>
-      <c r="F22" s="84"/>
-      <c r="G22" s="84"/>
-      <c r="H22" s="84"/>
-      <c r="I22" s="84"/>
-      <c r="J22" s="84"/>
-      <c r="K22" s="84"/>
-      <c r="L22" s="84"/>
-      <c r="M22" s="85"/>
-    </row>
-    <row r="23" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="87" t="s">
+      <c r="C22" s="87"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="87"/>
+      <c r="K22" s="87"/>
+      <c r="L22" s="87"/>
+      <c r="M22" s="88"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B23" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="88"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="87" t="s">
+      <c r="C23" s="84"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="88"/>
-      <c r="G23" s="89"/>
-      <c r="H23" s="87" t="s">
+      <c r="F23" s="84"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="83" t="s">
         <v>114</v>
       </c>
-      <c r="I23" s="88"/>
-      <c r="J23" s="89"/>
-      <c r="K23" s="87" t="s">
+      <c r="I23" s="84"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="L23" s="88"/>
-      <c r="M23" s="89"/>
+      <c r="L23" s="84"/>
+      <c r="M23" s="85"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
@@ -7841,12 +7838,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B22:M22"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="M13:N13"/>
@@ -7855,6 +7846,12 @@
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B22:M22"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:G10">
     <cfRule type="dataBar" priority="44">
@@ -8304,7 +8301,7 @@
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>nacht</v>
+        <v>more</v>
       </c>
       <c r="D2" t="e">
         <f t="shared" ref="D2:D7" ca="1" si="0">_xlfn.CONCAT(B2,C2)</f>
@@ -8323,7 +8320,7 @@
         <v>8</v>
       </c>
       <c r="H2" t="e">
-        <f ca="1">_xlfn.XLOOKUP(B2,Table2[Name],Table2[Ability 12])</f>
+        <f ca="1">_xlfn.XLOOKUP(B2,Table2[Name],Table2[Ability 1])</f>
         <v>#REF!</v>
       </c>
       <c r="I2" t="str">
@@ -8336,7 +8333,7 @@
       </c>
       <c r="K2" t="str" cm="1">
         <f t="array" aca="1" ref="K2" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Dima</v>
+        <v>Ultra</v>
       </c>
       <c r="L2" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
@@ -8373,7 +8370,7 @@
       </c>
       <c r="C3" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>line</v>
+        <v>bium</v>
       </c>
       <c r="D3" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8392,7 +8389,7 @@
         <v>8</v>
       </c>
       <c r="H3" t="e">
-        <f ca="1">_xlfn.XLOOKUP(B3,Table2[Name],Table2[Ability 12])</f>
+        <f ca="1">_xlfn.XLOOKUP(B3,Table2[Name],Table2[Ability 1])</f>
         <v>#REF!</v>
       </c>
       <c r="I3" t="str">
@@ -8405,7 +8402,7 @@
       </c>
       <c r="K3" t="str" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Supra</v>
+        <v>Meta</v>
       </c>
       <c r="L3" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
@@ -8442,7 +8439,7 @@
       </c>
       <c r="C4" t="str" cm="1">
         <f t="array" aca="1" ref="C4" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>talus</v>
+        <v>mant</v>
       </c>
       <c r="D4" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8461,7 +8458,7 @@
         <v>8</v>
       </c>
       <c r="H4" t="e">
-        <f ca="1">_xlfn.XLOOKUP(B4,Table2[Name],Table2[Ability 12])</f>
+        <f ca="1">_xlfn.XLOOKUP(B4,Table2[Name],Table2[Ability 1])</f>
         <v>#REF!</v>
       </c>
       <c r="I4" t="str">
@@ -8474,11 +8471,11 @@
       </c>
       <c r="K4" t="str" cm="1">
         <f t="array" aca="1" ref="K4" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Meta</v>
+        <v>Blasta</v>
       </c>
       <c r="L4" t="str" cm="1">
         <f t="array" aca="1" ref="L4" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Shello</v>
+        <v>Giga</v>
       </c>
       <c r="M4" t="e">
         <f ca="1">SUM(Table8[[#This Row],[Cost]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Cost]))</f>
@@ -8511,7 +8508,7 @@
       </c>
       <c r="C5" t="str" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>ton</v>
+        <v>lus</v>
       </c>
       <c r="D5" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8530,7 +8527,7 @@
         <v>8</v>
       </c>
       <c r="H5" t="e">
-        <f ca="1">_xlfn.XLOOKUP(B5,Table2[Name],Table2[Ability 12])</f>
+        <f ca="1">_xlfn.XLOOKUP(B5,Table2[Name],Table2[Ability 1])</f>
         <v>#REF!</v>
       </c>
       <c r="I5" t="str">
@@ -8543,7 +8540,7 @@
       </c>
       <c r="K5" t="str" cm="1">
         <f t="array" aca="1" ref="K5" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Multi</v>
+        <v>Turbo</v>
       </c>
       <c r="L5" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
@@ -8580,7 +8577,7 @@
       </c>
       <c r="C6" t="str" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>ctos</v>
+        <v>saurus</v>
       </c>
       <c r="D6" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8599,7 +8596,7 @@
         <v>8</v>
       </c>
       <c r="H6" t="e">
-        <f ca="1">_xlfn.XLOOKUP(B6,Table2[Name],Table2[Ability 12])</f>
+        <f ca="1">_xlfn.XLOOKUP(B6,Table2[Name],Table2[Ability 1])</f>
         <v>#REF!</v>
       </c>
       <c r="I6" t="str">
@@ -8612,7 +8609,7 @@
       </c>
       <c r="K6" t="str" cm="1">
         <f t="array" aca="1" ref="K6" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Giga</v>
+        <v>Multi</v>
       </c>
       <c r="L6" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
@@ -8649,7 +8646,7 @@
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>byte</v>
+        <v>dome</v>
       </c>
       <c r="D7" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8668,7 +8665,7 @@
         <v>8</v>
       </c>
       <c r="H7" t="e">
-        <f ca="1">_xlfn.XLOOKUP(B7,Table2[Name],Table2[Ability 12])</f>
+        <f ca="1">_xlfn.XLOOKUP(B7,Table2[Name],Table2[Ability 1])</f>
         <v>#REF!</v>
       </c>
       <c r="I7" t="str">
@@ -8681,7 +8678,7 @@
       </c>
       <c r="K7" t="str" cm="1">
         <f t="array" aca="1" ref="K7" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Shello</v>
+        <v>Dima</v>
       </c>
       <c r="L7" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>

</xml_diff>

<commit_message>
"Implement AI. TODO: Fix action search; throws 'single positional indexer is out-of-bounds' error when matching action in action list."
</commit_message>
<xml_diff>
--- a/Excel/BotBuilder 2.0.xlsx
+++ b/Excel/BotBuilder 2.0.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SJWDa\Projects\Fragment\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6CFC33-0D9B-4D47-AE47-24DFDFE90F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3B751E-50E6-4046-BF62-75C29B8B1E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{8281E10D-33EF-4D46-A534-1BAF9E624D7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8281E10D-33EF-4D46-A534-1BAF9E624D7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Passive abilities" sheetId="4" r:id="rId1"/>
-    <sheet name="Generator rules" sheetId="9" r:id="rId2"/>
-    <sheet name="Active abilities" sheetId="8" r:id="rId3"/>
-    <sheet name="Generators" sheetId="1" r:id="rId4"/>
-    <sheet name="Frames" sheetId="2" r:id="rId5"/>
-    <sheet name="Parts" sheetId="3" r:id="rId6"/>
-    <sheet name="Power Configuration" sheetId="7" r:id="rId7"/>
-    <sheet name="Bots" sheetId="6" r:id="rId8"/>
-    <sheet name="Statuses" sheetId="5" r:id="rId9"/>
+    <sheet name="Abilities" sheetId="10" r:id="rId2"/>
+    <sheet name="Generator rules" sheetId="9" r:id="rId3"/>
+    <sheet name="Active abilities" sheetId="8" r:id="rId4"/>
+    <sheet name="Generators" sheetId="1" r:id="rId5"/>
+    <sheet name="Frames" sheetId="2" r:id="rId6"/>
+    <sheet name="Parts" sheetId="3" r:id="rId7"/>
+    <sheet name="Power Configuration" sheetId="7" r:id="rId8"/>
+    <sheet name="Bots" sheetId="6" r:id="rId9"/>
+    <sheet name="Statuses" sheetId="5" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="Abilities">'Passive abilities'!$A$1:$C$24</definedName>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="268">
   <si>
     <t>Name</t>
   </si>
@@ -884,7 +885,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1000,8 +1001,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1212,8 +1221,20 @@
         <bgColor rgb="FFDDEBF7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1358,11 +1379,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1448,15 +1482,6 @@
     <xf numFmtId="0" fontId="8" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1469,11 +1494,277 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="91">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2261,246 +2552,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2731,16 +2782,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2774,17 +2815,17 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{CFB70296-300F-41E9-B29C-A15C0D2E492E}" name="Table15" displayName="Table15" ref="L14:O20" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{CFB70296-300F-41E9-B29C-A15C0D2E492E}" name="Table15" displayName="Table15" ref="L14:O20" totalsRowShown="0" headerRowDxfId="41" tableBorderDxfId="40">
   <autoFilter ref="L14:O20" xr:uid="{CFB70296-300F-41E9-B29C-A15C0D2E492E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{67B9F3DD-84E5-4E12-9557-0E15E2E8CD01}" name="Type" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{882509E9-98E0-4845-9863-913DA546EA5B}" name="Cost" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{67B9F3DD-84E5-4E12-9557-0E15E2E8CD01}" name="Type" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{882509E9-98E0-4845-9863-913DA546EA5B}" name="Cost" dataDxfId="38">
       <calculatedColumnFormula>ROUND(2*SUMIF(Cost_Stat[Type],Table15[[#This Row],[Type]],Cost_Stat[Actual9]),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8E6F0F0A-DEBA-4962-9C42-B7696451440A}" name="HP" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{8E6F0F0A-DEBA-4962-9C42-B7696451440A}" name="HP" dataDxfId="37">
       <calculatedColumnFormula>Table15[[#This Row],[Cost]]*SUMIF(Cost_Stat[Type],Table15[[#This Row],[Type]],Cost_Stat[Actual])/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8646B895-6FEE-4C10-AE30-8852BA384EB5}" name="PP" dataDxfId="11">
+    <tableColumn id="8" xr3:uid="{8646B895-6FEE-4C10-AE30-8852BA384EB5}" name="PP" dataDxfId="36">
       <calculatedColumnFormula>Table15[[#This Row],[Cost]]*SUMIF(Cost_Stat[Type],Table15[[#This Row],[Type]],Cost_Stat[Actual3])/2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2797,16 +2838,16 @@
   <autoFilter ref="A1:Q7" xr:uid="{3FAA1044-8AEB-4310-B12B-1961BF440AB5}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{ABACA6C5-D5B7-485A-BC77-3A9C1EF55782}" name="Type"/>
-    <tableColumn id="2" xr3:uid="{98DBF1C9-36B3-457C-864F-594F9B4A43F9}" name="Generator" dataDxfId="10">
+    <tableColumn id="2" xr3:uid="{98DBF1C9-36B3-457C-864F-594F9B4A43F9}" name="Generator" dataDxfId="35">
       <calculatedColumnFormula array="1">INDEX(Table2[Name],LARGE(IF(#REF!=Table8[[#This Row],[Type]],ROW(#REF!)-1),INT(RAND()*COUNTIF(#REF!,Table8[[#This Row],[Type]])+1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FC5D1622-0FC8-4A00-8958-9A4F98C2C4A3}" name="Frame" dataDxfId="9">
+    <tableColumn id="3" xr3:uid="{FC5D1622-0FC8-4A00-8958-9A4F98C2C4A3}" name="Frame" dataDxfId="34">
       <calculatedColumnFormula array="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{DB7035C1-3C3A-4574-9174-299FCD6046BE}" name="Name">
       <calculatedColumnFormula>_xlfn.CONCAT(B2,C2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B5ED832F-A98B-4E4D-B1BF-CEFAFBF20091}" name="Cost" dataDxfId="8">
+    <tableColumn id="9" xr3:uid="{B5ED832F-A98B-4E4D-B1BF-CEFAFBF20091}" name="Cost" dataDxfId="33">
       <calculatedColumnFormula>SUM(_xlfn.XLOOKUP(Table8[[#This Row],[Generator]],Table2[Name],Table2[Cost]),_xlfn.XLOOKUP(Table8[[#This Row],[Frame]],Table1[Name],Table1[Cost]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{5FBA6BAB-A94C-4CA0-A545-F10CD5101759}" name="PP">
@@ -2821,28 +2862,28 @@
     <tableColumn id="8" xr3:uid="{D892DF1C-8138-4EB4-8C4C-A6F7B91F63C4}" name="Ability 2">
       <calculatedColumnFormula>_xlfn.XLOOKUP(C2,Table1[Name],Table1[Action 1])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{621F2675-DA39-4950-BD2E-A247E9053807}" name="Power/Cost" dataDxfId="7">
+    <tableColumn id="16" xr3:uid="{621F2675-DA39-4950-BD2E-A247E9053807}" name="Power/Cost" dataDxfId="32">
       <calculatedColumnFormula>(Table8[[#This Row],[PP]]+(Table8[[#This Row],[HP]]/2)+IF(Table8[[#This Row],[Ability 1]]=0,0,1)+IF(Table8[[#This Row],[Ability 2]]=0,0,1))/(Table8[[#This Row],[Cost]]+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1043AF08-BB57-45E8-B3CF-7FB7430E40B1}" name="Part 1" dataDxfId="6">
+    <tableColumn id="10" xr3:uid="{1043AF08-BB57-45E8-B3CF-7FB7430E40B1}" name="Part 1" dataDxfId="31">
       <calculatedColumnFormula array="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{109CDE57-0F48-4932-B7BE-EAE14DBBDEB2}" name="Name2" dataDxfId="5">
+    <tableColumn id="11" xr3:uid="{109CDE57-0F48-4932-B7BE-EAE14DBBDEB2}" name="Name2" dataDxfId="30">
       <calculatedColumnFormula>_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{61864B2F-DDDC-4DBA-890D-CE1EC3F23BE7}" name="Cost2" dataDxfId="4">
+    <tableColumn id="12" xr3:uid="{61864B2F-DDDC-4DBA-890D-CE1EC3F23BE7}" name="Cost2" dataDxfId="29">
       <calculatedColumnFormula>SUM(Table8[[#This Row],[Cost]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Cost]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{FECCECFA-E3F9-4DA5-9AC1-015032FEDEB9}" name="PP2" dataDxfId="3">
+    <tableColumn id="13" xr3:uid="{FECCECFA-E3F9-4DA5-9AC1-015032FEDEB9}" name="PP2" dataDxfId="28">
       <calculatedColumnFormula>SUM(Table8[[#This Row],[PP]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Action]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6E9D2E4F-4D5A-4E1E-91F4-22754FFFE3CC}" name="HP2" dataDxfId="2">
+    <tableColumn id="14" xr3:uid="{6E9D2E4F-4D5A-4E1E-91F4-22754FFFE3CC}" name="HP2" dataDxfId="27">
       <calculatedColumnFormula>SUM(Table8[[#This Row],[HP]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[HP]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{BCBD232D-B15D-4401-9CF2-DC0F3D6CC7D1}" name="Ability" dataDxfId="1">
+    <tableColumn id="15" xr3:uid="{BCBD232D-B15D-4401-9CF2-DC0F3D6CC7D1}" name="Ability" dataDxfId="26">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{AFEF4760-EB7A-4908-B1B6-2F830AC5F848}" name="Power/Cost2" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{AFEF4760-EB7A-4908-B1B6-2F830AC5F848}" name="Power/Cost2" dataDxfId="25">
       <calculatedColumnFormula>(Table8[[#This Row],[PP2]]+(Table8[[#This Row],[HP2]]/2)+IF(Table8[[#This Row],[Ability 1]]=0,0,1)+IF(Table8[[#This Row],[Ability 2]]=0,0,1))/(Table8[[#This Row],[Cost]]+1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2862,11 +2903,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{62FD676D-EB53-4F49-8BF9-E2089D28B6B0}" name="Table7" displayName="Table7" ref="I7:J14" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{62FD676D-EB53-4F49-8BF9-E2089D28B6B0}" name="Table7" displayName="Table7" ref="I7:J14" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89">
   <autoFilter ref="I7:J14" xr:uid="{62FD676D-EB53-4F49-8BF9-E2089D28B6B0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{4B17C9F4-98B4-4E1A-A341-A45A31B8E33B}" name="Resource" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{4318EB6E-AE10-4D55-8A19-126C2931DF94}" name="Abilities" dataDxfId="86">
+    <tableColumn id="1" xr3:uid="{4B17C9F4-98B4-4E1A-A341-A45A31B8E33B}" name="Resource" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{4318EB6E-AE10-4D55-8A19-126C2931DF94}" name="Abilities" dataDxfId="87">
       <calculatedColumnFormula>COUNTIF(Table4[Resource],I8)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2884,7 +2925,7 @@
     <tableColumn id="1" xr3:uid="{EFE17165-DF3C-41D5-82FE-D4D71327F108}" name="Active Ability"/>
     <tableColumn id="3" xr3:uid="{ED842C65-134C-4739-9504-8A5630C40034}" name="Type"/>
     <tableColumn id="2" xr3:uid="{78127444-FC3B-4ACD-989C-698DAD1C2122}" name="Cost"/>
-    <tableColumn id="4" xr3:uid="{94D5DE63-FE7C-4B38-BA54-0FEAE4D293FA}" name="Effect" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{94D5DE63-FE7C-4B38-BA54-0FEAE4D293FA}" name="Effect" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2895,10 +2936,10 @@
   <autoFilter ref="A1:E43" xr:uid="{7A4F3B76-8375-4FD9-8128-9BF9E8EECA3E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{44860EA4-FD5F-4598-AEEF-F7BFC26B7043}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{7AB76467-159E-460D-9139-B4222C9E583D}" name="Deck" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{7AB76467-159E-460D-9139-B4222C9E583D}" name="Deck" dataDxfId="85"/>
     <tableColumn id="3" xr3:uid="{E017E39D-29F1-4E55-98B2-8FC221A535CB}" name="Cost"/>
     <tableColumn id="4" xr3:uid="{0C4B96A8-AEC8-4A0E-8BE8-D7CB34749D2F}" name="HP"/>
-    <tableColumn id="6" xr3:uid="{C3850DEF-7805-4A9E-9633-EEEB17887BC8}" name="Ability 1" dataDxfId="83"/>
+    <tableColumn id="6" xr3:uid="{C3850DEF-7805-4A9E-9633-EEEB17887BC8}" name="Ability 1" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2923,38 +2964,38 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BD6F9D4F-C6DA-4DA9-9AF2-B383883F498D}" name="Table3" displayName="Table3" ref="A1:D16" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BD6F9D4F-C6DA-4DA9-9AF2-B383883F498D}" name="Table3" displayName="Table3" ref="A1:D16" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="A1:D16" xr:uid="{BD6F9D4F-C6DA-4DA9-9AF2-B383883F498D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{98031720-D200-46F3-9ACA-C1755FECC5FB}" name="Name" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{EF26975E-EC1C-434E-9124-8EA3E2771B2B}" name="Cost" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{B5C3D5E2-952F-4B3E-9501-9A5F8E406832}" name="HP" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{91393694-5AF1-4A22-906A-4DDEB27DF551}" name="Action" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{98031720-D200-46F3-9ACA-C1755FECC5FB}" name="Name" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{EF26975E-EC1C-434E-9124-8EA3E2771B2B}" name="Cost" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{B5C3D5E2-952F-4B3E-9501-9A5F8E406832}" name="HP" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{91393694-5AF1-4A22-906A-4DDEB27DF551}" name="Action" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{AC6516ED-FA98-4523-83EE-69A55ECFF39F}" name="Variety" displayName="Variety" ref="A4:G10" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{AC6516ED-FA98-4523-83EE-69A55ECFF39F}" name="Variety" displayName="Variety" ref="A4:G10" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
   <autoFilter ref="A4:G10" xr:uid="{AC6516ED-FA98-4523-83EE-69A55ECFF39F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:G10">
     <sortCondition ref="A4:A10"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0D866C81-1CAB-4FD7-97E5-8378FE482ECB}" name="Type" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{9A9DEA20-92D8-4011-950B-D6302196503D}" name="Ideal" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{1C762ECE-0C98-4920-B0E4-55A7A19F83FE}" name="Actual" dataDxfId="48">
+    <tableColumn id="1" xr3:uid="{0D866C81-1CAB-4FD7-97E5-8378FE482ECB}" name="Type" dataDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{9A9DEA20-92D8-4011-950B-D6302196503D}" name="Ideal" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{1C762ECE-0C98-4920-B0E4-55A7A19F83FE}" name="Actual" dataDxfId="73">
       <calculatedColumnFormula>COUNTIF(Table1[Deck],Variety[[#This Row],[Type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0C8BE51C-0A54-4ED3-B98C-1D7DB953F369}" name="Difference" dataDxfId="47">
+    <tableColumn id="4" xr3:uid="{0C8BE51C-0A54-4ED3-B98C-1D7DB953F369}" name="Difference" dataDxfId="72">
       <calculatedColumnFormula>C5-B5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{3AED6875-DAF4-4906-BE77-76EDD3B57540}" name="Ideal2" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{2038FDEC-12A5-484F-BDCE-984800935EE8}" name="Actual3" dataDxfId="45">
+    <tableColumn id="5" xr3:uid="{3AED6875-DAF4-4906-BE77-76EDD3B57540}" name="Ideal2" dataDxfId="71"/>
+    <tableColumn id="6" xr3:uid="{2038FDEC-12A5-484F-BDCE-984800935EE8}" name="Actual3" dataDxfId="70">
       <calculatedColumnFormula>COUNTIF(#REF!,Variety[[#This Row],[Type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F7D4ECF7-C059-4A05-99E4-7061721663F5}" name="Difference4" dataDxfId="44">
+    <tableColumn id="7" xr3:uid="{F7D4ECF7-C059-4A05-99E4-7061721663F5}" name="Difference4" dataDxfId="69">
       <calculatedColumnFormula>F5-E5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2963,32 +3004,32 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{0A7EB303-0E7F-45E7-8409-4BDD8FBA1748}" name="Stats" displayName="Stats" ref="A14:J20" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{0A7EB303-0E7F-45E7-8409-4BDD8FBA1748}" name="Stats" displayName="Stats" ref="A14:J20" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
   <autoFilter ref="A14:J20" xr:uid="{0A7EB303-0E7F-45E7-8409-4BDD8FBA1748}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:J20">
     <sortCondition ref="A14:A20"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{7EB7684E-4D07-449A-BFD3-43839697E526}" name="Type" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{75578D46-0A1F-4356-BCA2-A452E28A1417}" name="Ideal" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{B17B7A7F-D00A-4E52-B2CF-783A8BDD18B4}" name="Actual" dataDxfId="39">
+    <tableColumn id="1" xr3:uid="{7EB7684E-4D07-449A-BFD3-43839697E526}" name="Type" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{75578D46-0A1F-4356-BCA2-A452E28A1417}" name="Ideal" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{B17B7A7F-D00A-4E52-B2CF-783A8BDD18B4}" name="Actual" dataDxfId="64">
       <calculatedColumnFormula>SUMIF(Table1[Deck],Stats[[#This Row],[Type]],Table1[HP])/COUNTIF(Table1[Deck],Stats[[#This Row],[Type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A3CF985F-4F0F-467E-93FF-CB89776629BB}" name="Difference" dataDxfId="38">
+    <tableColumn id="4" xr3:uid="{A3CF985F-4F0F-467E-93FF-CB89776629BB}" name="Difference" dataDxfId="63">
       <calculatedColumnFormula>C15-B15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8BFB7AA2-1B75-4F79-966A-74B6F8ED5B7F}" name="Ideal2" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{BE17EF79-FC56-4637-9C8B-66F29560F811}" name="Actual3" dataDxfId="36">
+    <tableColumn id="5" xr3:uid="{8BFB7AA2-1B75-4F79-966A-74B6F8ED5B7F}" name="Ideal2" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{BE17EF79-FC56-4637-9C8B-66F29560F811}" name="Actual3" dataDxfId="61">
       <calculatedColumnFormula array="1">SUMIF(#REF!,Stats[[#This Row],[Type]],Table2[HP])/COUNTIF(#REF!,Stats[[#This Row],[Type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{583ABFEB-99E8-4030-BFD2-685DD430FA80}" name="Difference4" dataDxfId="35">
+    <tableColumn id="7" xr3:uid="{583ABFEB-99E8-4030-BFD2-685DD430FA80}" name="Difference4" dataDxfId="60">
       <calculatedColumnFormula>F15-E15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B3A60430-2211-48DF-B47C-68AE8FB6A2BB}" name="Ideal5" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{E6BC29A1-559E-44E9-A302-CE348EC0B5D9}" name="Actual6" dataDxfId="33">
+    <tableColumn id="8" xr3:uid="{B3A60430-2211-48DF-B47C-68AE8FB6A2BB}" name="Ideal5" dataDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{E6BC29A1-559E-44E9-A302-CE348EC0B5D9}" name="Actual6" dataDxfId="58">
       <calculatedColumnFormula>(SUMIF(Table1[Deck],Stats[[#This Row],[Type]],Table1[Action 2])+SUMIF(#REF!,Stats[[#This Row],[Type]],#REF!))/(COUNTIF(Table1[Deck],Stats[[#This Row],[Type]])+COUNTIF(#REF!,Stats[[#This Row],[Type]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5E66CDD0-39AD-4632-9676-0BF8F6414C7E}" name="Difference7" dataDxfId="32">
+    <tableColumn id="10" xr3:uid="{5E66CDD0-39AD-4632-9676-0BF8F6414C7E}" name="Difference7" dataDxfId="57">
       <calculatedColumnFormula>I15-H15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2997,39 +3038,39 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{D9B208C6-E117-47B0-B9C7-9A034FB99F5B}" name="Cost_Stat" displayName="Cost_Stat" ref="A24:M30" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{D9B208C6-E117-47B0-B9C7-9A034FB99F5B}" name="Cost_Stat" displayName="Cost_Stat" ref="A24:M30" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
   <autoFilter ref="A24:M30" xr:uid="{D9B208C6-E117-47B0-B9C7-9A034FB99F5B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:M30">
     <sortCondition ref="A24:A30"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{F7B32CDF-9BB4-47AF-BE3F-842F7D6EF736}" name="Type" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{E517E5F7-276F-406B-A78C-73C12B03024A}" name="Ideal" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{54CFC0BE-CB89-4B6F-9EA5-3D4D0425EF87}" name="Actual" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{F7B32CDF-9BB4-47AF-BE3F-842F7D6EF736}" name="Type" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{E517E5F7-276F-406B-A78C-73C12B03024A}" name="Ideal" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{54CFC0BE-CB89-4B6F-9EA5-3D4D0425EF87}" name="Actual" dataDxfId="52">
       <calculatedColumnFormula>SUMIF(Table1[Deck],Cost_Stat[[#This Row],[Type]],Table1[HP])/SUMIF(Table1[Deck],Cost_Stat[[#This Row],[Type]],Table1[Cost])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{485B5A87-DD44-4B1F-95C2-F593EAB7581E}" name="Difference" dataDxfId="26">
+    <tableColumn id="4" xr3:uid="{485B5A87-DD44-4B1F-95C2-F593EAB7581E}" name="Difference" dataDxfId="51">
       <calculatedColumnFormula>C25-B25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{0AB55B04-7DB1-4B3B-95A0-41BE01235610}" name="Ideal2" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{EBE0B5B1-010C-4B8E-BF94-291D680A295E}" name="Actual3" dataDxfId="24">
+    <tableColumn id="5" xr3:uid="{0AB55B04-7DB1-4B3B-95A0-41BE01235610}" name="Ideal2" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{EBE0B5B1-010C-4B8E-BF94-291D680A295E}" name="Actual3" dataDxfId="49">
       <calculatedColumnFormula>SUMIF(#REF!,Cost_Stat[[#This Row],[Type]],Table2[HP])/SUMIF(#REF!,Cost_Stat[[#This Row],[Type]],Table2[Cost])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{DF4CF3C4-B12B-46B7-BC59-E5351C495BC1}" name="Difference4" dataDxfId="23">
+    <tableColumn id="7" xr3:uid="{DF4CF3C4-B12B-46B7-BC59-E5351C495BC1}" name="Difference4" dataDxfId="48">
       <calculatedColumnFormula>F25-E25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{466E32FE-7121-4644-899F-C08F4CE38771}" name="Ideal5" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{FF597456-2300-4BC6-8B64-D1A298F13E5A}" name="Actual6" dataDxfId="21">
+    <tableColumn id="8" xr3:uid="{466E32FE-7121-4644-899F-C08F4CE38771}" name="Ideal5" dataDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{FF597456-2300-4BC6-8B64-D1A298F13E5A}" name="Actual6" dataDxfId="46">
       <calculatedColumnFormula>(SUMIF(Table1[Deck],Cost_Stat[[#This Row],[Type]],Table1[Action 2])+SUMIF(#REF!,Cost_Stat[[#This Row],[Type]],#REF!))/(SUMIFS(Table1[Cost],Table1[Deck],Cost_Stat[[#This Row],[Type]],Table1[Action 2],1)+SUMIFS(Table2[Cost],#REF!,Cost_Stat[[#This Row],[Type]],#REF!,1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{FB0F2832-C6B6-4855-8222-A7A9323ACFC9}" name="Difference7" dataDxfId="20">
+    <tableColumn id="10" xr3:uid="{FB0F2832-C6B6-4855-8222-A7A9323ACFC9}" name="Difference7" dataDxfId="45">
       <calculatedColumnFormula>I25-H25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{73909C54-2246-4ED8-B808-E4BE1DD4A485}" name="Ideal8" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{2B1962BE-7805-4FFA-8D3C-E67730E4E5EA}" name="Actual9" dataDxfId="18">
+    <tableColumn id="11" xr3:uid="{73909C54-2246-4ED8-B808-E4BE1DD4A485}" name="Ideal8" dataDxfId="44"/>
+    <tableColumn id="12" xr3:uid="{2B1962BE-7805-4FFA-8D3C-E67730E4E5EA}" name="Actual9" dataDxfId="43">
       <calculatedColumnFormula>(SUMIF(Table1[Deck],Cost_Stat[[#This Row],[Type]],Table1[Cost])+SUMIF(#REF!,Cost_Stat[[#This Row],[Type]],Table2[Cost]))/(COUNTIF(Table1[Deck],Cost_Stat[[#This Row],[Type]])+COUNTIF(#REF!,Cost_Stat[[#This Row],[Type]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{05006522-125E-42FB-A202-48124F65E1AF}" name="Difference10" dataDxfId="17">
+    <tableColumn id="13" xr3:uid="{05006522-125E-42FB-A202-48124F65E1AF}" name="Difference10" dataDxfId="42">
       <calculatedColumnFormula>L25-K25</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3337,7 +3378,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="D36" sqref="A1:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4061,7 +4102,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E36">
-    <cfRule type="cellIs" dxfId="90" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4074,7 +4115,489 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBABE18-0F7C-4B0E-8916-623B8CDA6BE4}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CC94AC-604E-4A7D-A764-8AA6F7CED8E9}">
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="92" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="93" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="93" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="90" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="91" t="str">
+        <f>"-1 PP to draw a card once per turn"</f>
+        <v>-1 PP to draw a card once per turn</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="95" t="str">
+        <f>"-1 PP to upgrade a bot"</f>
+        <v>-1 PP to upgrade a bot</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="90" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="91" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="91" t="str">
+        <f>"-1 PP to swap a new resource once per turn"</f>
+        <v>-1 PP to swap a new resource once per turn</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="94" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="95" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="95" t="str">
+        <f>"-1 PP to move a bot once per turn"</f>
+        <v>-1 PP to move a bot once per turn</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="90" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="91" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="91" t="str">
+        <f>"-1 PP to build a bot"</f>
+        <v>-1 PP to build a bot</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="94" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="95" t="str">
+        <f>"-1 PP to power a bot"</f>
+        <v>-1 PP to power a bot</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="90" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="91" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="91" t="str">
+        <f>"-1 PP to play mechanic cards"</f>
+        <v>-1 PP to play mechanic cards</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="94" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="95" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="95" t="str">
+        <f>"+2 HP each time you draw a card"</f>
+        <v>+2 HP each time you draw a card</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="91" t="str">
+        <f>"+2 HP each time an ally bot is upgraded"</f>
+        <v>+2 HP each time an ally bot is upgraded</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="94" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="95" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="95" t="str">
+        <f>"+2 HP each time you mine a new resource"</f>
+        <v>+2 HP each time you mine a new resource</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="90" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" s="91" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="91" t="str">
+        <f>"+2 HP each time a bot moves"</f>
+        <v>+2 HP each time a bot moves</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="94" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="95" t="str">
+        <f>"+2 HP each time a new bot is built"</f>
+        <v>+2 HP each time a new bot is built</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="90" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="91" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="91" t="str">
+        <f>"+2 HP each time you power a bot"</f>
+        <v>+2 HP each time you power a bot</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="94" t="s">
+        <v>183</v>
+      </c>
+      <c r="B15" s="95" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="95" t="str">
+        <f>"+2 HP each time you play a mechanic card"</f>
+        <v>+2 HP each time you play a mechanic card</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="90" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="91" t="str">
+        <f>"+2 PP whenever an opponent draws a card"</f>
+        <v>+2 PP whenever an opponent draws a card</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="94" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="95" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="95" t="str">
+        <f>"+2 PP whenever an opponent upgrades a bot"</f>
+        <v>+2 PP whenever an opponent upgrades a bot</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="90" t="s">
+        <v>184</v>
+      </c>
+      <c r="B18" s="91" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="91" t="str">
+        <f>"+2 PP whenever an opponent mines a resource"</f>
+        <v>+2 PP whenever an opponent mines a resource</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="94" t="s">
+        <v>187</v>
+      </c>
+      <c r="B19" s="95" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="95" t="str">
+        <f>"+2 PP whenever an opponent moves a bot"</f>
+        <v>+2 PP whenever an opponent moves a bot</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="90" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" s="91" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="91" t="str">
+        <f>"+2 PP whenever an opponent builds a bot"</f>
+        <v>+2 PP whenever an opponent builds a bot</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="94" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="95" t="str">
+        <f>"+2 PP whenever an opponent powers a bot"</f>
+        <v>+2 PP whenever an opponent powers a bot</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="90" t="s">
+        <v>188</v>
+      </c>
+      <c r="B22" s="91" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" s="91" t="str">
+        <f>"+2 PP whenever an opponent plays a mechanic card"</f>
+        <v>+2 PP whenever an opponent plays a mechanic card</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="94" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="95" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="95" t="str">
+        <f>"+1 PP whenever opponent bot gains HP"</f>
+        <v>+1 PP whenever opponent bot gains HP</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="90" t="s">
+        <v>165</v>
+      </c>
+      <c r="B24" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="91" t="str">
+        <f>"+1 PP per turn for each upgrade on this bot"</f>
+        <v>+1 PP per turn for each upgrade on this bot</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="94" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" s="95" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="95" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="90" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="91" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="96" t="str">
+        <f>"+1 PP from each non-adjacent Weather Event resource"</f>
+        <v>+1 PP from each non-adjacent Weather Event resource</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="94" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="95" t="str">
+        <f>"+1 PP each turn for each active friendly bot"</f>
+        <v>+1 PP each turn for each active friendly bot</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="90" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" s="91" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="91" t="str">
+        <f>"+2 PP each time a friendly bot is destroyed"</f>
+        <v>+2 PP each time a friendly bot is destroyed</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="94" t="s">
+        <v>178</v>
+      </c>
+      <c r="B29" s="95" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" s="95" t="str">
+        <f>"+2 PP each time an enemy bot is destroyed"</f>
+        <v>+2 PP each time an enemy bot is destroyed</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="90" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="91" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="94" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="95" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="95" t="str">
+        <f>"+1 dmg dealt for each upgrade on this bot"</f>
+        <v>+1 dmg dealt for each upgrade on this bot</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="90" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="91" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="91" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="94" t="s">
+        <v>180</v>
+      </c>
+      <c r="B33" s="95" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="95" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="90" t="s">
+        <v>149</v>
+      </c>
+      <c r="B34" s="91" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="91" t="str">
+        <f>"+1 dmg to attacks for each bot you destroy"</f>
+        <v>+1 dmg to attacks for each bot you destroy</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="94" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="95" t="str">
+        <f>"-1 dmg to each attack against this bot"</f>
+        <v>-1 dmg to each attack against this bot</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="90" t="s">
+        <v>179</v>
+      </c>
+      <c r="B36" s="91" t="s">
+        <v>173</v>
+      </c>
+      <c r="C36" s="91" t="str">
+        <f>"+1 effect for mechanic cards"</f>
+        <v>+1 effect for mechanic cards</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7CFDD3E-3930-40B7-B7D3-BAB54582CA32}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -4163,7 +4686,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DCEAB9-AE33-4163-9970-7E135343EEE1}">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -4410,11 +4933,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A60404A-0BD4-4949-BF8C-296F3D670006}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -5305,7 +5828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F33C8B6-3B38-4842-B741-8602A8A78BF0}">
   <dimension ref="A1:F57"/>
   <sheetViews>
@@ -5323,7 +5846,7 @@
     <col min="8" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -6471,7 +6994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E8417B-6ED1-4BDA-A68A-01122B3E11CB}">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -6718,7 +7241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74A5B2D-9A7D-4116-841E-BBD1252B93F2}">
   <dimension ref="A1:O30"/>
   <sheetViews>
@@ -6745,34 +7268,34 @@
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="88"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="85"/>
       <c r="H2" s="14"/>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="83" t="s">
         <v>144</v>
       </c>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="88"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="85"/>
       <c r="M2" s="14"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B3" s="83" t="s">
+    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="83" t="s">
+      <c r="C3" s="88"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="87" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="84"/>
-      <c r="G3" s="85"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="89"/>
       <c r="H3" s="15"/>
       <c r="I3" s="39" t="s">
         <v>111</v>
@@ -6830,7 +7353,7 @@
       </c>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>66</v>
       </c>
@@ -6911,7 +7434,7 @@
       </c>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>7</v>
       </c>
@@ -7048,40 +7571,40 @@
     </row>
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="86" t="s">
+      <c r="B12" s="83" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="88"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="85"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B13" s="83" t="s">
+    <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="84"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="83" t="s">
+      <c r="C13" s="88"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="84"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="83" t="s">
+      <c r="F13" s="88"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="I13" s="84"/>
-      <c r="J13" s="85"/>
+      <c r="I13" s="88"/>
+      <c r="J13" s="89"/>
       <c r="K13" s="38"/>
-      <c r="M13" s="89"/>
-      <c r="N13" s="89"/>
+      <c r="M13" s="86"/>
+      <c r="N13" s="86"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -7464,42 +7987,42 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="86" t="s">
+      <c r="B22" s="83" t="s">
         <v>129</v>
       </c>
-      <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="87"/>
-      <c r="I22" s="87"/>
-      <c r="J22" s="87"/>
-      <c r="K22" s="87"/>
-      <c r="L22" s="87"/>
-      <c r="M22" s="88"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B23" s="83" t="s">
+      <c r="C22" s="84"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="84"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="84"/>
+      <c r="K22" s="84"/>
+      <c r="L22" s="84"/>
+      <c r="M22" s="85"/>
+    </row>
+    <row r="23" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B23" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="84"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="83" t="s">
+      <c r="C23" s="88"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="84"/>
-      <c r="G23" s="85"/>
-      <c r="H23" s="83" t="s">
+      <c r="F23" s="88"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="I23" s="84"/>
-      <c r="J23" s="85"/>
-      <c r="K23" s="83" t="s">
+      <c r="I23" s="88"/>
+      <c r="J23" s="89"/>
+      <c r="K23" s="87" t="s">
         <v>130</v>
       </c>
-      <c r="L23" s="84"/>
-      <c r="M23" s="85"/>
+      <c r="L23" s="88"/>
+      <c r="M23" s="89"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
@@ -7838,6 +8361,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B22:M22"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="M13:N13"/>
@@ -7846,12 +8375,6 @@
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:G3"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B22:M22"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:G10">
     <cfRule type="dataBar" priority="44">
@@ -7978,62 +8501,62 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A10">
-    <cfRule type="cellIs" dxfId="76" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="36" operator="equal">
       <formula>"Preserve"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="37" operator="equal">
       <formula>"Cultivate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="38" operator="equal">
       <formula>"Convert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="39" operator="equal">
       <formula>"Consume"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="40" operator="equal">
       <formula>"Augment"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="41" operator="equal">
       <formula>"Acquire"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:A20">
-    <cfRule type="cellIs" dxfId="70" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="30" operator="equal">
       <formula>"Preserve"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="31" operator="equal">
       <formula>"Cultivate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="32" operator="equal">
       <formula>"Convert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="33" operator="equal">
       <formula>"Consume"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="34" operator="equal">
       <formula>"Augment"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="35" operator="equal">
       <formula>"Acquire"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:A30">
-    <cfRule type="cellIs" dxfId="64" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="18" operator="equal">
       <formula>"Preserve"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
       <formula>"Cultivate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="20" operator="equal">
       <formula>"Convert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="21" operator="equal">
       <formula>"Consume"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="22" operator="equal">
       <formula>"Augment"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="23" operator="equal">
       <formula>"Acquire"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8108,22 +8631,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15:L20">
-    <cfRule type="cellIs" dxfId="58" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Preserve"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Cultivate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"Convert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"Consume"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"Augment"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>"Acquire"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8221,7 +8744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67FE3AA-5974-40EC-BB86-435967AC9781}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
@@ -8301,7 +8824,7 @@
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>more</v>
+        <v>klum</v>
       </c>
       <c r="D2" t="e">
         <f t="shared" ref="D2:D7" ca="1" si="0">_xlfn.CONCAT(B2,C2)</f>
@@ -8333,7 +8856,7 @@
       </c>
       <c r="K2" t="str" cm="1">
         <f t="array" aca="1" ref="K2" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Ultra</v>
+        <v>Supra</v>
       </c>
       <c r="L2" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
@@ -8370,7 +8893,7 @@
       </c>
       <c r="C3" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>bium</v>
+        <v>zine</v>
       </c>
       <c r="D3" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8402,7 +8925,7 @@
       </c>
       <c r="K3" t="str" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Meta</v>
+        <v>Multi</v>
       </c>
       <c r="L3" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
@@ -8439,7 +8962,7 @@
       </c>
       <c r="C4" t="str" cm="1">
         <f t="array" aca="1" ref="C4" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>mant</v>
+        <v>nax</v>
       </c>
       <c r="D4" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8471,11 +8994,11 @@
       </c>
       <c r="K4" t="str" cm="1">
         <f t="array" aca="1" ref="K4" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Blasta</v>
+        <v>Turbo</v>
       </c>
       <c r="L4" t="str" cm="1">
         <f t="array" aca="1" ref="L4" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Giga</v>
+        <v>Meta</v>
       </c>
       <c r="M4" t="e">
         <f ca="1">SUM(Table8[[#This Row],[Cost]],_xlfn.XLOOKUP(Table8[[#This Row],[Part 1]],Table3[Name],Table3[Cost]))</f>
@@ -8508,7 +9031,7 @@
       </c>
       <c r="C5" t="str" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>lus</v>
+        <v>bar</v>
       </c>
       <c r="D5" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8540,7 +9063,7 @@
       </c>
       <c r="K5" t="str" cm="1">
         <f t="array" aca="1" ref="K5" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Turbo</v>
+        <v>Ultra</v>
       </c>
       <c r="L5" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
@@ -8577,7 +9100,7 @@
       </c>
       <c r="C6" t="str" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>saurus</v>
+        <v>lophus</v>
       </c>
       <c r="D6" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8609,7 +9132,7 @@
       </c>
       <c r="K6" t="str" cm="1">
         <f t="array" aca="1" ref="K6" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Multi</v>
+        <v>Ultra</v>
       </c>
       <c r="L6" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
@@ -8646,7 +9169,7 @@
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">INDEX(Table1[Name],LARGE(IF(Table1[Deck]=Table8[[#This Row],[Type]],ROW(Table1[Deck])-1),INT(RAND()*COUNTIF(Table1[Deck],Table8[[#This Row],[Type]])+1)))</f>
-        <v>dome</v>
+        <v>lite</v>
       </c>
       <c r="D7" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8678,7 +9201,7 @@
       </c>
       <c r="K7" t="str" cm="1">
         <f t="array" aca="1" ref="K7" ca="1">INDEX(Table3[Name],INT(RAND()*COUNTA(Table3[Name])+1))</f>
-        <v>Dima</v>
+        <v>Meta</v>
       </c>
       <c r="L7" t="e">
         <f ca="1">_xlfn.CONCAT(Table8[[#This Row],[Generator]],Table8[[#This Row],[Part 1]],Table8[[#This Row],[Frame]])</f>
@@ -8736,44 +9259,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBABE18-0F7C-4B0E-8916-623B8CDA6BE4}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>